<commit_message>
Jk added header again so code will run
</commit_message>
<xml_diff>
--- a/data/OC Coho Abundance.xlsx
+++ b/data/OC Coho Abundance.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/oliviasomhegyi/Desktop/Grad School/GP/SalmonStocks/github/salmon_sisters/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BDED5E7-C5D8-E547-9EAE-A81D5AC7348F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7D69F78-547B-914B-B46D-093730D4670C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="28">
   <si>
     <t>Year</t>
   </si>
@@ -116,6 +116,9 @@
   </si>
   <si>
     <t>WILD COHO HARVEST ESTIMATES</t>
+  </si>
+  <si>
+    <t>TOTAL WILD ABUNDANCE</t>
   </si>
 </sst>
 </file>
@@ -1008,10 +1011,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:V31"/>
+  <dimension ref="A1:V32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1030,2110 +1033,2115 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="2" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A2" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B2" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="C2" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="D2" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="7" t="s">
+      <c r="E2" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="7" t="s">
+      <c r="F2" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="7" t="s">
+      <c r="G2" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="7" t="s">
+      <c r="H2" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="7" t="s">
+      <c r="I2" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="7" t="s">
+      <c r="J2" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="7" t="s">
+      <c r="K2" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="7" t="s">
+      <c r="L2" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="7" t="s">
+      <c r="M2" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="7" t="s">
+      <c r="N2" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="7" t="s">
+      <c r="O2" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="7" t="s">
+      <c r="P2" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="7" t="s">
+      <c r="Q2" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="7" t="s">
+      <c r="R2" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="S1" s="7" t="s">
+      <c r="S2" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="T1" s="7" t="s">
+      <c r="T2" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="U1" s="7" t="s">
+      <c r="U2" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="V1" s="7" t="s">
+      <c r="V2" s="7" t="s">
         <v>21</v>
-      </c>
-    </row>
-    <row r="2" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A2" s="1">
-        <v>1994</v>
-      </c>
-      <c r="B2" s="1">
-        <v>878</v>
-      </c>
-      <c r="C2" s="1">
-        <v>716</v>
-      </c>
-      <c r="D2" s="1">
-        <v>15370</v>
-      </c>
-      <c r="E2" s="1">
-        <v>5426</v>
-      </c>
-      <c r="F2" s="1">
-        <v>2812</v>
-      </c>
-      <c r="G2" s="1">
-        <v>2928</v>
-      </c>
-      <c r="H2" s="1">
-        <v>2292</v>
-      </c>
-      <c r="I2" s="1">
-        <v>285</v>
-      </c>
-      <c r="J2" s="1">
-        <v>3015</v>
-      </c>
-      <c r="K2" s="1">
-        <v>282</v>
-      </c>
-      <c r="L2" s="1">
-        <v>953</v>
-      </c>
-      <c r="M2" s="1">
-        <v>96</v>
-      </c>
-      <c r="N2" s="1">
-        <v>658</v>
-      </c>
-      <c r="O2" s="1">
-        <v>1380</v>
-      </c>
-      <c r="P2" s="1">
-        <v>3349</v>
-      </c>
-      <c r="Q2" s="1">
-        <v>252</v>
-      </c>
-      <c r="R2" s="1">
-        <v>1146</v>
-      </c>
-      <c r="S2" s="1">
-        <v>1119</v>
-      </c>
-      <c r="T2" s="1">
-        <v>3555</v>
-      </c>
-      <c r="U2" s="1">
-        <v>1171</v>
-      </c>
-      <c r="V2" s="1">
-        <v>2162</v>
       </c>
     </row>
     <row r="3" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
-        <v>1995</v>
+        <v>1994</v>
       </c>
       <c r="B3" s="1">
-        <v>490</v>
+        <v>878</v>
       </c>
       <c r="C3" s="1">
-        <v>342</v>
+        <v>716</v>
       </c>
       <c r="D3" s="1">
-        <v>11435</v>
+        <v>15370</v>
       </c>
       <c r="E3" s="1">
-        <v>2258</v>
+        <v>5426</v>
       </c>
       <c r="F3" s="1">
-        <v>1500</v>
+        <v>2812</v>
       </c>
       <c r="G3" s="1">
-        <v>12048</v>
+        <v>2928</v>
       </c>
       <c r="H3" s="1">
-        <v>3608</v>
+        <v>2292</v>
       </c>
       <c r="I3" s="1">
-        <v>201</v>
+        <v>285</v>
       </c>
       <c r="J3" s="1">
-        <v>1887</v>
+        <v>3015</v>
       </c>
       <c r="K3" s="1">
-        <v>1706</v>
+        <v>282</v>
       </c>
       <c r="L3" s="1">
-        <v>1435</v>
+        <v>953</v>
       </c>
       <c r="M3" s="1">
-        <v>117</v>
+        <v>96</v>
       </c>
       <c r="N3" s="1">
-        <v>349</v>
+        <v>658</v>
       </c>
       <c r="O3" s="1">
-        <v>4901</v>
+        <v>1380</v>
       </c>
       <c r="P3" s="1">
-        <v>6839</v>
+        <v>3349</v>
       </c>
       <c r="Q3" s="1">
-        <v>85</v>
+        <v>252</v>
       </c>
       <c r="R3" s="1">
-        <v>5234</v>
+        <v>1146</v>
       </c>
       <c r="S3" s="1">
-        <v>1750</v>
+        <v>1119</v>
       </c>
       <c r="T3" s="1">
-        <v>5652</v>
+        <v>3555</v>
       </c>
       <c r="U3" s="1">
-        <v>379</v>
+        <v>1171</v>
       </c>
       <c r="V3" s="1">
-        <v>5243</v>
+        <v>2162</v>
       </c>
     </row>
     <row r="4" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
-        <v>1996</v>
+        <v>1995</v>
       </c>
       <c r="B4" s="1">
-        <v>1124</v>
+        <v>490</v>
       </c>
       <c r="C4" s="1">
-        <v>1374</v>
+        <v>342</v>
       </c>
       <c r="D4" s="1">
-        <v>12856</v>
+        <v>11435</v>
       </c>
       <c r="E4" s="1">
-        <v>16763</v>
+        <v>2258</v>
       </c>
       <c r="F4" s="1">
-        <v>1610</v>
+        <v>1500</v>
       </c>
       <c r="G4" s="1">
-        <v>8464</v>
+        <v>12048</v>
       </c>
       <c r="H4" s="1">
-        <v>5391</v>
+        <v>3608</v>
       </c>
       <c r="I4" s="1">
-        <v>441</v>
+        <v>201</v>
       </c>
       <c r="J4" s="1">
-        <v>559</v>
+        <v>1887</v>
       </c>
       <c r="K4" s="1">
-        <v>466</v>
+        <v>1706</v>
       </c>
       <c r="L4" s="1">
-        <v>1133</v>
+        <v>1435</v>
       </c>
       <c r="M4" s="1">
-        <v>87</v>
+        <v>117</v>
       </c>
       <c r="N4" s="1">
-        <v>419</v>
+        <v>349</v>
       </c>
       <c r="O4" s="1">
-        <v>4989</v>
+        <v>4901</v>
       </c>
       <c r="P4" s="1">
-        <v>7668</v>
+        <v>6839</v>
       </c>
       <c r="Q4" s="1">
-        <v>206</v>
+        <v>85</v>
       </c>
       <c r="R4" s="1">
-        <v>7462</v>
+        <v>5234</v>
       </c>
       <c r="S4" s="1">
-        <v>1725</v>
+        <v>1750</v>
       </c>
       <c r="T4" s="1">
-        <v>7518</v>
+        <v>5652</v>
       </c>
       <c r="U4" s="1">
-        <v>777</v>
+        <v>379</v>
       </c>
       <c r="V4" s="1">
-        <v>4853</v>
+        <v>5243</v>
       </c>
     </row>
     <row r="5" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
-        <v>1997</v>
+        <v>1996</v>
       </c>
       <c r="B5" s="1">
-        <v>655</v>
+        <v>1124</v>
       </c>
       <c r="C5" s="1">
-        <v>542</v>
+        <v>1374</v>
       </c>
       <c r="D5" s="1">
-        <v>1212</v>
+        <v>12856</v>
       </c>
       <c r="E5" s="1">
-        <v>6235</v>
+        <v>16763</v>
       </c>
       <c r="F5" s="1">
-        <v>525</v>
+        <v>1610</v>
       </c>
       <c r="G5" s="1">
-        <v>1370</v>
+        <v>8464</v>
       </c>
       <c r="H5" s="1">
-        <v>614</v>
+        <v>5391</v>
       </c>
       <c r="I5" s="1">
-        <v>106</v>
+        <v>441</v>
       </c>
       <c r="J5" s="1">
-        <v>1294</v>
+        <v>559</v>
       </c>
       <c r="K5" s="1">
-        <v>251</v>
+        <v>466</v>
       </c>
       <c r="L5" s="1">
-        <v>629</v>
+        <v>1133</v>
       </c>
       <c r="M5" s="1">
-        <v>17</v>
+        <v>87</v>
       </c>
       <c r="N5" s="1">
-        <v>325</v>
+        <v>419</v>
       </c>
       <c r="O5" s="1">
-        <v>2892</v>
+        <v>4989</v>
       </c>
       <c r="P5" s="1">
-        <v>546</v>
+        <v>7668</v>
       </c>
       <c r="Q5" s="1">
-        <v>156</v>
+        <v>206</v>
       </c>
       <c r="R5" s="1">
-        <v>1021</v>
+        <v>7462</v>
       </c>
       <c r="S5" s="1">
-        <v>2008</v>
+        <v>1725</v>
       </c>
       <c r="T5" s="1">
-        <v>4460</v>
+        <v>7518</v>
       </c>
       <c r="U5" s="1">
-        <v>476</v>
+        <v>777</v>
       </c>
       <c r="V5" s="1">
-        <v>457</v>
+        <v>4853</v>
       </c>
     </row>
     <row r="6" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
-        <v>1998</v>
+        <v>1997</v>
       </c>
       <c r="B6" s="1">
-        <v>117</v>
+        <v>655</v>
       </c>
       <c r="C6" s="1">
-        <v>433</v>
+        <v>542</v>
       </c>
       <c r="D6" s="1">
-        <v>3224</v>
+        <v>1212</v>
       </c>
       <c r="E6" s="1">
-        <v>2605</v>
+        <v>6235</v>
       </c>
       <c r="F6" s="1">
-        <v>949</v>
+        <v>525</v>
       </c>
       <c r="G6" s="1">
-        <v>4916</v>
+        <v>1370</v>
       </c>
       <c r="H6" s="1">
-        <v>1358</v>
+        <v>614</v>
       </c>
       <c r="I6" s="1">
-        <v>621</v>
+        <v>106</v>
       </c>
       <c r="J6" s="1">
-        <v>1302</v>
+        <v>1294</v>
       </c>
       <c r="K6" s="1">
-        <v>218</v>
+        <v>251</v>
       </c>
       <c r="L6" s="1">
-        <v>826</v>
+        <v>629</v>
       </c>
       <c r="M6" s="1">
-        <v>93</v>
+        <v>17</v>
       </c>
       <c r="N6" s="1">
-        <v>341</v>
+        <v>325</v>
       </c>
       <c r="O6" s="1">
-        <v>3372</v>
+        <v>2892</v>
       </c>
       <c r="P6" s="1">
-        <v>1102</v>
+        <v>546</v>
       </c>
       <c r="Q6" s="1">
-        <v>603</v>
+        <v>156</v>
       </c>
       <c r="R6" s="1">
-        <v>3431</v>
+        <v>1021</v>
       </c>
       <c r="S6" s="1">
-        <v>3042</v>
+        <v>2008</v>
       </c>
       <c r="T6" s="1">
-        <v>5583</v>
+        <v>4460</v>
       </c>
       <c r="U6" s="1">
-        <v>387</v>
+        <v>476</v>
       </c>
       <c r="V6" s="1">
-        <v>551</v>
+        <v>457</v>
       </c>
     </row>
     <row r="7" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
-        <v>1999</v>
+        <v>1998</v>
       </c>
       <c r="B7" s="1">
-        <v>1435</v>
+        <v>117</v>
       </c>
       <c r="C7" s="1">
-        <v>1617</v>
+        <v>433</v>
       </c>
       <c r="D7" s="1">
-        <v>5155</v>
+        <v>3224</v>
       </c>
       <c r="E7" s="1">
-        <v>2854</v>
+        <v>2605</v>
       </c>
       <c r="F7" s="1">
-        <v>717</v>
+        <v>949</v>
       </c>
       <c r="G7" s="1">
-        <v>2807</v>
+        <v>4916</v>
       </c>
       <c r="H7" s="1">
-        <v>1870</v>
+        <v>1358</v>
       </c>
       <c r="I7" s="1">
-        <v>376</v>
+        <v>621</v>
       </c>
       <c r="J7" s="1">
-        <v>3804</v>
+        <v>1302</v>
       </c>
       <c r="K7" s="1">
-        <v>2522</v>
+        <v>218</v>
       </c>
       <c r="L7" s="1">
-        <v>1278</v>
+        <v>826</v>
       </c>
       <c r="M7" s="1">
-        <v>15</v>
+        <v>93</v>
       </c>
       <c r="N7" s="1">
-        <v>1294</v>
+        <v>341</v>
       </c>
       <c r="O7" s="1">
-        <v>2949</v>
+        <v>3372</v>
       </c>
       <c r="P7" s="1">
-        <v>3189</v>
+        <v>1102</v>
       </c>
       <c r="Q7" s="1">
-        <v>60</v>
+        <v>603</v>
       </c>
       <c r="R7" s="1">
-        <v>3222</v>
+        <v>3431</v>
       </c>
       <c r="S7" s="1">
-        <v>3920</v>
+        <v>3042</v>
       </c>
       <c r="T7" s="1">
-        <v>6552</v>
+        <v>5583</v>
       </c>
       <c r="U7" s="1">
-        <v>1959</v>
+        <v>387</v>
       </c>
       <c r="V7" s="1">
-        <v>2742</v>
+        <v>551</v>
       </c>
     </row>
     <row r="8" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
-        <v>2000</v>
+        <v>1999</v>
       </c>
       <c r="B8" s="1">
-        <v>3498</v>
+        <v>1435</v>
       </c>
       <c r="C8" s="1">
-        <v>1523</v>
+        <v>1617</v>
       </c>
       <c r="D8" s="1">
-        <v>4892</v>
+        <v>5155</v>
       </c>
       <c r="E8" s="1">
-        <v>6503</v>
+        <v>2854</v>
       </c>
       <c r="F8" s="1">
-        <v>1536</v>
+        <v>717</v>
       </c>
       <c r="G8" s="1">
-        <v>6012</v>
+        <v>2807</v>
       </c>
       <c r="H8" s="1">
-        <v>4737</v>
+        <v>1870</v>
       </c>
       <c r="I8" s="1">
-        <v>373</v>
+        <v>376</v>
       </c>
       <c r="J8" s="1">
-        <v>15040</v>
+        <v>3804</v>
       </c>
       <c r="K8" s="1">
-        <v>1268</v>
+        <v>2522</v>
       </c>
       <c r="L8" s="1">
-        <v>1744</v>
+        <v>1278</v>
       </c>
       <c r="M8" s="1">
-        <v>186</v>
+        <v>15</v>
       </c>
       <c r="N8" s="1">
-        <v>3522</v>
+        <v>1294</v>
       </c>
       <c r="O8" s="1">
-        <v>3988</v>
+        <v>2949</v>
       </c>
       <c r="P8" s="1">
-        <v>6793</v>
+        <v>3189</v>
       </c>
       <c r="Q8" s="1">
-        <v>141</v>
+        <v>60</v>
       </c>
       <c r="R8" s="1">
-        <v>2684</v>
+        <v>3222</v>
       </c>
       <c r="S8" s="1">
-        <v>659</v>
+        <v>3920</v>
       </c>
       <c r="T8" s="1">
-        <v>8609</v>
+        <v>6552</v>
       </c>
       <c r="U8" s="1">
-        <v>2265</v>
+        <v>1959</v>
       </c>
       <c r="V8" s="1">
-        <v>662</v>
+        <v>2742</v>
       </c>
     </row>
     <row r="9" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
-        <v>2001</v>
+        <v>2000</v>
       </c>
       <c r="B9" s="1">
-        <v>3357</v>
+        <v>3498</v>
       </c>
       <c r="C9" s="1">
-        <v>1905</v>
+        <v>1523</v>
       </c>
       <c r="D9" s="1">
-        <v>34939</v>
+        <v>4892</v>
       </c>
       <c r="E9" s="1">
-        <v>14386</v>
+        <v>6503</v>
       </c>
       <c r="F9" s="1">
-        <v>5891</v>
+        <v>1536</v>
       </c>
       <c r="G9" s="1">
-        <v>12105</v>
+        <v>6012</v>
       </c>
       <c r="H9" s="1">
-        <v>9298</v>
+        <v>4737</v>
       </c>
       <c r="I9" s="1">
-        <v>5025</v>
+        <v>373</v>
       </c>
       <c r="J9" s="1">
-        <v>22805</v>
+        <v>15040</v>
       </c>
       <c r="K9" s="1">
-        <v>4331</v>
+        <v>1268</v>
       </c>
       <c r="L9" s="1">
-        <v>2739</v>
+        <v>1744</v>
       </c>
       <c r="M9" s="1">
-        <v>234</v>
+        <v>186</v>
       </c>
       <c r="N9" s="1">
-        <v>1659</v>
+        <v>3522</v>
       </c>
       <c r="O9" s="1">
-        <v>5308</v>
+        <v>3988</v>
       </c>
       <c r="P9" s="1">
-        <v>11030</v>
+        <v>6793</v>
       </c>
       <c r="Q9" s="1">
-        <v>99</v>
+        <v>141</v>
       </c>
       <c r="R9" s="1">
-        <v>12346</v>
+        <v>2684</v>
       </c>
       <c r="S9" s="1">
-        <v>3650</v>
+        <v>659</v>
       </c>
       <c r="T9" s="1">
-        <v>11430</v>
+        <v>8609</v>
       </c>
       <c r="U9" s="1">
-        <v>2022</v>
+        <v>2265</v>
       </c>
       <c r="V9" s="1">
-        <v>3733</v>
+        <v>662</v>
       </c>
     </row>
     <row r="10" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
-        <v>2002</v>
+        <v>2001</v>
       </c>
       <c r="B10" s="1">
-        <v>9527</v>
+        <v>3357</v>
       </c>
       <c r="C10" s="1">
-        <v>3378</v>
+        <v>1905</v>
       </c>
       <c r="D10" s="1">
-        <v>34776</v>
+        <v>34939</v>
       </c>
       <c r="E10" s="1">
-        <v>8060</v>
+        <v>14386</v>
       </c>
       <c r="F10" s="1">
-        <v>3436</v>
+        <v>5891</v>
       </c>
       <c r="G10" s="1">
-        <v>19825</v>
+        <v>12105</v>
       </c>
       <c r="H10" s="1">
-        <v>11275</v>
+        <v>9298</v>
       </c>
       <c r="I10" s="1">
-        <v>2149</v>
+        <v>5025</v>
       </c>
       <c r="J10" s="1">
-        <v>18022</v>
+        <v>22805</v>
       </c>
       <c r="K10" s="1">
-        <v>17533</v>
+        <v>4331</v>
       </c>
       <c r="L10" s="1">
-        <v>3536</v>
+        <v>2739</v>
       </c>
       <c r="M10" s="1">
-        <v>570</v>
+        <v>234</v>
       </c>
       <c r="N10" s="1">
-        <v>2235</v>
+        <v>1659</v>
       </c>
       <c r="O10" s="1">
-        <v>4868</v>
+        <v>5308</v>
       </c>
       <c r="P10" s="1">
-        <v>58217</v>
+        <v>11030</v>
       </c>
       <c r="Q10" s="1">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="R10" s="1">
-        <v>11043</v>
+        <v>12346</v>
       </c>
       <c r="S10" s="1">
-        <v>3654</v>
+        <v>3650</v>
       </c>
       <c r="T10" s="1">
-        <v>14554</v>
+        <v>11430</v>
       </c>
       <c r="U10" s="1">
-        <v>14001</v>
+        <v>2022</v>
       </c>
       <c r="V10" s="1">
-        <v>24990</v>
+        <v>3733</v>
       </c>
     </row>
     <row r="11" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
-        <v>2003</v>
+        <v>2002</v>
       </c>
       <c r="B11" s="1">
-        <v>11103</v>
+        <v>9527</v>
       </c>
       <c r="C11" s="1">
-        <v>5996</v>
+        <v>3378</v>
       </c>
       <c r="D11" s="1">
-        <v>27822</v>
+        <v>34776</v>
       </c>
       <c r="E11" s="1">
-        <v>24195</v>
+        <v>8060</v>
       </c>
       <c r="F11" s="1">
-        <v>1028</v>
+        <v>3436</v>
       </c>
       <c r="G11" s="1">
-        <v>17814</v>
+        <v>19825</v>
       </c>
       <c r="H11" s="1">
-        <v>11977</v>
+        <v>11275</v>
       </c>
       <c r="I11" s="1">
-        <v>2567</v>
+        <v>2149</v>
       </c>
       <c r="J11" s="1">
-        <v>35118</v>
+        <v>18022</v>
       </c>
       <c r="K11" s="1">
-        <v>11010</v>
+        <v>17533</v>
       </c>
       <c r="L11" s="1">
-        <v>3091</v>
+        <v>3536</v>
       </c>
       <c r="M11" s="1">
-        <v>45</v>
+        <v>570</v>
       </c>
       <c r="N11" s="1">
-        <v>8681</v>
+        <v>2235</v>
       </c>
       <c r="O11" s="1">
-        <v>7158</v>
+        <v>4868</v>
       </c>
       <c r="P11" s="1">
-        <v>31323</v>
+        <v>58217</v>
       </c>
       <c r="Q11" s="1">
-        <v>93</v>
+        <v>100</v>
       </c>
       <c r="R11" s="1">
-        <v>4684</v>
+        <v>11043</v>
       </c>
       <c r="S11" s="1">
-        <v>3443</v>
+        <v>3654</v>
       </c>
       <c r="T11" s="1">
-        <v>6761</v>
+        <v>14554</v>
       </c>
       <c r="U11" s="1">
-        <v>14049</v>
+        <v>14001</v>
       </c>
       <c r="V11" s="1">
-        <v>17803</v>
+        <v>24990</v>
       </c>
     </row>
     <row r="12" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
-        <v>2004</v>
+        <v>2003</v>
       </c>
       <c r="B12" s="1">
-        <v>5652</v>
+        <v>11103</v>
       </c>
       <c r="C12" s="1">
-        <v>4935</v>
+        <v>5996</v>
       </c>
       <c r="D12" s="1">
-        <v>25204</v>
+        <v>27822</v>
       </c>
       <c r="E12" s="1">
-        <v>23909</v>
+        <v>24195</v>
       </c>
       <c r="F12" s="1">
-        <v>8042</v>
+        <v>1028</v>
       </c>
       <c r="G12" s="1">
-        <v>9708</v>
+        <v>17814</v>
       </c>
       <c r="H12" s="1">
-        <v>6885</v>
+        <v>11977</v>
       </c>
       <c r="I12" s="1">
-        <v>2374</v>
+        <v>2567</v>
       </c>
       <c r="J12" s="1">
-        <v>20235</v>
+        <v>35118</v>
       </c>
       <c r="K12" s="1">
-        <v>5071</v>
+        <v>11010</v>
       </c>
       <c r="L12" s="1">
-        <v>3844</v>
+        <v>3091</v>
       </c>
       <c r="M12" s="1">
-        <v>1773</v>
+        <v>45</v>
       </c>
       <c r="N12" s="1">
-        <v>8833</v>
+        <v>8681</v>
       </c>
       <c r="O12" s="1">
-        <v>8638</v>
+        <v>7158</v>
       </c>
       <c r="P12" s="1">
-        <v>9427</v>
+        <v>31323</v>
       </c>
       <c r="Q12" s="1">
-        <v>435</v>
+        <v>93</v>
       </c>
       <c r="R12" s="1">
-        <v>11877</v>
+        <v>4684</v>
       </c>
       <c r="S12" s="1">
-        <v>3776</v>
+        <v>3443</v>
       </c>
       <c r="T12" s="1">
-        <v>7720</v>
+        <v>6761</v>
       </c>
       <c r="U12" s="1">
-        <v>2735</v>
+        <v>14049</v>
       </c>
       <c r="V12" s="1">
-        <v>5982</v>
+        <v>17803</v>
       </c>
     </row>
     <row r="13" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A13" s="1">
-        <v>2005</v>
+        <v>2004</v>
       </c>
       <c r="B13" s="1">
-        <v>14463</v>
+        <v>5652</v>
       </c>
       <c r="C13" s="1">
-        <v>2355</v>
+        <v>4935</v>
       </c>
       <c r="D13" s="1">
-        <v>17730</v>
+        <v>25204</v>
       </c>
       <c r="E13" s="1">
-        <v>12278</v>
+        <v>23909</v>
       </c>
       <c r="F13" s="1">
-        <v>526</v>
+        <v>8042</v>
       </c>
       <c r="G13" s="1">
-        <v>19335</v>
+        <v>9708</v>
       </c>
       <c r="H13" s="1">
-        <v>7912</v>
+        <v>6885</v>
       </c>
       <c r="I13" s="1">
-        <v>1267</v>
+        <v>2374</v>
       </c>
       <c r="J13" s="1">
-        <v>10869</v>
+        <v>20235</v>
       </c>
       <c r="K13" s="1">
-        <v>713</v>
+        <v>5071</v>
       </c>
       <c r="L13" s="1">
-        <v>2048</v>
+        <v>3844</v>
       </c>
       <c r="M13" s="1">
-        <v>82</v>
+        <v>1773</v>
       </c>
       <c r="N13" s="1">
-        <v>15150</v>
+        <v>8833</v>
       </c>
       <c r="O13" s="1">
-        <v>4539</v>
+        <v>8638</v>
       </c>
       <c r="P13" s="1">
-        <v>17583</v>
+        <v>9427</v>
       </c>
       <c r="Q13" s="1">
-        <v>109</v>
+        <v>435</v>
       </c>
       <c r="R13" s="1">
-        <v>14939</v>
+        <v>11877</v>
       </c>
       <c r="S13" s="1">
-        <v>1973</v>
+        <v>3776</v>
       </c>
       <c r="T13" s="1">
-        <v>8803</v>
+        <v>7720</v>
       </c>
       <c r="U13" s="1">
-        <v>2075</v>
+        <v>2735</v>
       </c>
       <c r="V13" s="1">
-        <v>3579</v>
+        <v>5982</v>
       </c>
     </row>
     <row r="14" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A14" s="1">
-        <v>2006</v>
+        <v>2005</v>
       </c>
       <c r="B14" s="1">
-        <v>2130</v>
+        <v>14463</v>
       </c>
       <c r="C14" s="1">
-        <v>2106</v>
+        <v>2355</v>
       </c>
       <c r="D14" s="1">
-        <v>12167</v>
+        <v>17730</v>
       </c>
       <c r="E14" s="1">
-        <v>30863</v>
+        <v>12278</v>
       </c>
       <c r="F14" s="1">
-        <v>1192</v>
+        <v>526</v>
       </c>
       <c r="G14" s="1">
-        <v>8634</v>
+        <v>19335</v>
       </c>
       <c r="H14" s="1">
-        <v>5240</v>
+        <v>7912</v>
       </c>
       <c r="I14" s="1">
-        <v>810</v>
+        <v>1267</v>
       </c>
       <c r="J14" s="1">
-        <v>12543</v>
+        <v>10869</v>
       </c>
       <c r="K14" s="1">
-        <v>2026</v>
+        <v>713</v>
       </c>
       <c r="L14" s="1">
-        <v>3240</v>
+        <v>2048</v>
       </c>
       <c r="M14" s="1">
-        <v>554</v>
+        <v>82</v>
       </c>
       <c r="N14" s="1">
-        <v>5621</v>
+        <v>15150</v>
       </c>
       <c r="O14" s="1">
-        <v>5888</v>
+        <v>4539</v>
       </c>
       <c r="P14" s="1">
-        <v>6339</v>
+        <v>17583</v>
       </c>
       <c r="Q14" s="1">
-        <v>318</v>
+        <v>109</v>
       </c>
       <c r="R14" s="1">
-        <v>2426</v>
+        <v>14939</v>
       </c>
       <c r="S14" s="1">
-        <v>3900</v>
+        <v>1973</v>
       </c>
       <c r="T14" s="1">
-        <v>16269</v>
+        <v>8803</v>
       </c>
       <c r="U14" s="1">
-        <v>9476</v>
+        <v>2075</v>
       </c>
       <c r="V14" s="1">
-        <v>4587</v>
+        <v>3579</v>
       </c>
     </row>
     <row r="15" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A15" s="1">
-        <v>2007</v>
+        <v>2006</v>
       </c>
       <c r="B15" s="1">
-        <v>2404</v>
+        <v>2130</v>
       </c>
       <c r="C15" s="1">
-        <v>684</v>
+        <v>2106</v>
       </c>
       <c r="D15" s="1">
-        <v>1488</v>
+        <v>12167</v>
       </c>
       <c r="E15" s="1">
-        <v>15644</v>
+        <v>30863</v>
       </c>
       <c r="F15" s="1">
-        <v>381</v>
+        <v>1192</v>
       </c>
       <c r="G15" s="1">
-        <v>4745</v>
+        <v>8634</v>
       </c>
       <c r="H15" s="1">
-        <v>1777</v>
+        <v>5240</v>
       </c>
       <c r="I15" s="1">
-        <v>483</v>
+        <v>810</v>
       </c>
       <c r="J15" s="1">
-        <v>15717</v>
+        <v>12543</v>
       </c>
       <c r="K15" s="1">
-        <v>441</v>
+        <v>2026</v>
       </c>
       <c r="L15" s="1">
-        <v>1579</v>
+        <v>3240</v>
       </c>
       <c r="M15" s="1">
-        <v>66</v>
+        <v>554</v>
       </c>
       <c r="N15" s="1">
-        <v>2461</v>
+        <v>5621</v>
       </c>
       <c r="O15" s="1">
-        <v>1621</v>
+        <v>5888</v>
       </c>
       <c r="P15" s="1">
-        <v>3978</v>
+        <v>6339</v>
       </c>
       <c r="Q15" s="1">
-        <v>109</v>
+        <v>318</v>
       </c>
       <c r="R15" s="1">
-        <v>5095</v>
+        <v>2426</v>
       </c>
       <c r="S15" s="1">
-        <v>3977</v>
+        <v>3900</v>
       </c>
       <c r="T15" s="1">
-        <v>4432</v>
+        <v>16269</v>
       </c>
       <c r="U15" s="1">
-        <v>2570</v>
+        <v>9476</v>
       </c>
       <c r="V15" s="1">
-        <v>3537</v>
+        <v>4587</v>
       </c>
     </row>
     <row r="16" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A16" s="1">
-        <v>2008</v>
+        <v>2007</v>
       </c>
       <c r="B16" s="1">
-        <v>13586</v>
+        <v>2404</v>
       </c>
       <c r="C16" s="1">
-        <v>1242</v>
+        <v>684</v>
       </c>
       <c r="D16" s="1">
-        <v>15179</v>
+        <v>1488</v>
       </c>
       <c r="E16" s="1">
-        <v>8967</v>
+        <v>15644</v>
       </c>
       <c r="F16" s="1">
-        <v>802</v>
+        <v>381</v>
       </c>
       <c r="G16" s="1">
-        <v>9203</v>
+        <v>4745</v>
       </c>
       <c r="H16" s="1">
-        <v>4561</v>
+        <v>1777</v>
       </c>
       <c r="I16" s="1">
-        <v>1076</v>
+        <v>483</v>
       </c>
       <c r="J16" s="1">
-        <v>17549</v>
+        <v>15717</v>
       </c>
       <c r="K16" s="1">
-        <v>1881</v>
+        <v>441</v>
       </c>
       <c r="L16" s="1">
-        <v>3507</v>
+        <v>1579</v>
       </c>
       <c r="M16" s="1">
-        <v>665</v>
+        <v>66</v>
       </c>
       <c r="N16" s="1">
-        <v>21047</v>
+        <v>2461</v>
       </c>
       <c r="O16" s="1">
-        <v>3950</v>
+        <v>1621</v>
       </c>
       <c r="P16" s="1">
-        <v>17841</v>
+        <v>3978</v>
       </c>
       <c r="Q16" s="1">
-        <v>44</v>
+        <v>109</v>
       </c>
       <c r="R16" s="1">
-        <v>21354</v>
+        <v>5095</v>
       </c>
       <c r="S16" s="1">
-        <v>2656</v>
+        <v>3977</v>
       </c>
       <c r="T16" s="1">
-        <v>17474</v>
+        <v>4432</v>
       </c>
       <c r="U16" s="1">
-        <v>4925</v>
+        <v>2570</v>
       </c>
       <c r="V16" s="1">
-        <v>11131</v>
+        <v>3537</v>
       </c>
     </row>
     <row r="17" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A17" s="1">
-        <v>2009</v>
+        <v>2008</v>
       </c>
       <c r="B17" s="1">
-        <v>15663</v>
+        <v>13586</v>
       </c>
       <c r="C17" s="1">
-        <v>3825</v>
+        <v>1242</v>
       </c>
       <c r="D17" s="1">
-        <v>28868</v>
+        <v>15179</v>
       </c>
       <c r="E17" s="1">
-        <v>23846</v>
+        <v>8967</v>
       </c>
       <c r="F17" s="1">
-        <v>3427</v>
+        <v>802</v>
       </c>
       <c r="G17" s="1">
-        <v>20592</v>
+        <v>9203</v>
       </c>
       <c r="H17" s="1">
-        <v>16130</v>
+        <v>4561</v>
       </c>
       <c r="I17" s="1">
-        <v>4095</v>
+        <v>1076</v>
       </c>
       <c r="J17" s="1">
-        <v>23276</v>
+        <v>17549</v>
       </c>
       <c r="K17" s="1">
-        <v>4550</v>
+        <v>1881</v>
       </c>
       <c r="L17" s="1">
-        <v>8260</v>
+        <v>3507</v>
       </c>
       <c r="M17" s="1">
-        <v>806</v>
+        <v>665</v>
       </c>
       <c r="N17" s="1">
-        <v>25755</v>
+        <v>21047</v>
       </c>
       <c r="O17" s="1">
-        <v>5561</v>
+        <v>3950</v>
       </c>
       <c r="P17" s="1">
-        <v>32749</v>
+        <v>17841</v>
       </c>
       <c r="Q17" s="1">
-        <v>188</v>
+        <v>44</v>
       </c>
       <c r="R17" s="1">
-        <v>17060</v>
+        <v>21354</v>
       </c>
       <c r="S17" s="1">
-        <v>3185</v>
+        <v>2656</v>
       </c>
       <c r="T17" s="1">
-        <v>9817</v>
+        <v>17474</v>
       </c>
       <c r="U17" s="1">
-        <v>17389</v>
+        <v>4925</v>
       </c>
       <c r="V17" s="1">
-        <v>11965</v>
+        <v>11131</v>
       </c>
     </row>
     <row r="18" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A18" s="1">
-        <v>2010</v>
+        <v>2009</v>
       </c>
       <c r="B18" s="1">
-        <v>10172</v>
+        <v>15663</v>
       </c>
       <c r="C18" s="1">
-        <v>2176</v>
+        <v>3825</v>
       </c>
       <c r="D18" s="1">
-        <v>29041</v>
+        <v>28868</v>
       </c>
       <c r="E18" s="1">
-        <v>24742</v>
+        <v>23846</v>
       </c>
       <c r="F18" s="1">
-        <v>11895</v>
+        <v>3427</v>
       </c>
       <c r="G18" s="1">
-        <v>18392</v>
+        <v>20592</v>
       </c>
       <c r="H18" s="1">
-        <v>19029</v>
+        <v>16130</v>
       </c>
       <c r="I18" s="1">
-        <v>4667</v>
+        <v>4095</v>
       </c>
       <c r="J18" s="1">
-        <v>33826</v>
+        <v>23276</v>
       </c>
       <c r="K18" s="1">
-        <v>2044</v>
+        <v>4550</v>
       </c>
       <c r="L18" s="1">
-        <v>9867</v>
+        <v>8260</v>
       </c>
       <c r="M18" s="1">
-        <v>1451</v>
+        <v>806</v>
       </c>
       <c r="N18" s="1">
-        <v>6597</v>
+        <v>25755</v>
       </c>
       <c r="O18" s="1">
-        <v>8062</v>
+        <v>5561</v>
       </c>
       <c r="P18" s="1">
-        <v>27282</v>
+        <v>32749</v>
       </c>
       <c r="Q18" s="1">
-        <v>97</v>
+        <v>188</v>
       </c>
       <c r="R18" s="1">
-        <v>26232</v>
+        <v>17060</v>
       </c>
       <c r="S18" s="1">
-        <v>11215</v>
+        <v>3185</v>
       </c>
       <c r="T18" s="1">
-        <v>21404</v>
+        <v>9817</v>
       </c>
       <c r="U18" s="1">
-        <v>15635</v>
+        <v>17389</v>
       </c>
       <c r="V18" s="1">
-        <v>9018</v>
+        <v>11965</v>
       </c>
     </row>
     <row r="19" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A19" s="1">
-        <v>2011</v>
+        <v>2010</v>
       </c>
       <c r="B19" s="1">
-        <v>30037</v>
+        <v>10172</v>
       </c>
       <c r="C19" s="1">
-        <v>2532</v>
+        <v>2176</v>
       </c>
       <c r="D19" s="1">
-        <v>11659</v>
+        <v>29041</v>
       </c>
       <c r="E19" s="1">
-        <v>59007</v>
+        <v>24742</v>
       </c>
       <c r="F19" s="1">
-        <v>9770</v>
+        <v>11895</v>
       </c>
       <c r="G19" s="1">
-        <v>19838</v>
+        <v>18392</v>
       </c>
       <c r="H19" s="1">
-        <v>21160</v>
+        <v>19029</v>
       </c>
       <c r="I19" s="1">
-        <v>2247</v>
+        <v>4667</v>
       </c>
       <c r="J19" s="1">
-        <v>16241</v>
+        <v>33826</v>
       </c>
       <c r="K19" s="1">
-        <v>8328</v>
+        <v>2044</v>
       </c>
       <c r="L19" s="1">
-        <v>6381</v>
+        <v>9867</v>
       </c>
       <c r="M19" s="1">
-        <v>3854</v>
+        <v>1451</v>
       </c>
       <c r="N19" s="1">
-        <v>35080</v>
+        <v>6597</v>
       </c>
       <c r="O19" s="1">
-        <v>6735</v>
+        <v>8062</v>
       </c>
       <c r="P19" s="1">
-        <v>29767</v>
+        <v>27282</v>
       </c>
       <c r="Q19" s="1">
-        <v>354</v>
+        <v>97</v>
       </c>
       <c r="R19" s="1">
-        <v>52955</v>
+        <v>26232</v>
       </c>
       <c r="S19" s="1">
-        <v>7043</v>
+        <v>11215</v>
       </c>
       <c r="T19" s="1">
-        <v>7721</v>
+        <v>21404</v>
       </c>
       <c r="U19" s="1">
-        <v>20405</v>
+        <v>15635</v>
       </c>
       <c r="V19" s="1">
-        <v>20218</v>
+        <v>9018</v>
       </c>
     </row>
     <row r="20" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A20" s="1">
-        <v>2012</v>
+        <v>2011</v>
       </c>
       <c r="B20" s="1">
-        <v>9995</v>
+        <v>30037</v>
       </c>
       <c r="C20" s="1">
-        <v>2216</v>
+        <v>2532</v>
       </c>
       <c r="D20" s="1">
-        <v>11109</v>
+        <v>11659</v>
       </c>
       <c r="E20" s="1">
-        <v>6975</v>
+        <v>59007</v>
       </c>
       <c r="F20" s="1">
-        <v>2952</v>
+        <v>9770</v>
       </c>
       <c r="G20" s="1">
-        <v>4403</v>
+        <v>19838</v>
       </c>
       <c r="H20" s="1">
-        <v>2887</v>
+        <v>21160</v>
       </c>
       <c r="I20" s="1">
-        <v>1064</v>
+        <v>2247</v>
       </c>
       <c r="J20" s="1">
-        <v>3496</v>
+        <v>16241</v>
       </c>
       <c r="K20" s="1">
-        <v>2066</v>
+        <v>8328</v>
       </c>
       <c r="L20" s="1">
-        <v>3698</v>
+        <v>6381</v>
       </c>
       <c r="M20" s="1">
-        <v>350</v>
+        <v>3854</v>
       </c>
       <c r="N20" s="1">
-        <v>5304</v>
+        <v>35080</v>
       </c>
       <c r="O20" s="1">
-        <v>4655</v>
+        <v>6735</v>
       </c>
       <c r="P20" s="1">
-        <v>14096</v>
+        <v>29767</v>
       </c>
       <c r="Q20" s="1">
-        <v>40</v>
+        <v>354</v>
       </c>
       <c r="R20" s="1">
-        <v>13730</v>
+        <v>52955</v>
       </c>
       <c r="S20" s="1">
-        <v>6697</v>
+        <v>7043</v>
       </c>
       <c r="T20" s="1">
-        <v>10976</v>
+        <v>7721</v>
       </c>
       <c r="U20" s="1">
-        <v>1989</v>
+        <v>20405</v>
       </c>
       <c r="V20" s="1">
-        <v>7396</v>
+        <v>20218</v>
       </c>
     </row>
     <row r="21" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A21" s="1">
-        <v>2013</v>
+        <v>2012</v>
       </c>
       <c r="B21" s="1">
-        <v>10583</v>
+        <v>9995</v>
       </c>
       <c r="C21" s="1">
-        <v>2297</v>
+        <v>2216</v>
       </c>
       <c r="D21" s="1">
-        <v>7848</v>
+        <v>11109</v>
       </c>
       <c r="E21" s="1">
-        <v>26946</v>
+        <v>6975</v>
       </c>
       <c r="F21" s="1">
-        <v>2207</v>
+        <v>2952</v>
       </c>
       <c r="G21" s="1">
-        <v>8883</v>
+        <v>4403</v>
       </c>
       <c r="H21" s="1">
-        <v>4870</v>
+        <v>2887</v>
       </c>
       <c r="I21" s="1">
-        <v>910</v>
+        <v>1064</v>
       </c>
       <c r="J21" s="1">
-        <v>5174</v>
+        <v>3496</v>
       </c>
       <c r="K21" s="1">
-        <v>1078</v>
+        <v>2066</v>
       </c>
       <c r="L21" s="1">
-        <v>3162</v>
+        <v>3698</v>
       </c>
       <c r="M21" s="1">
-        <v>1328</v>
+        <v>350</v>
       </c>
       <c r="N21" s="1">
-        <v>8732</v>
+        <v>5304</v>
       </c>
       <c r="O21" s="1">
-        <v>4329</v>
+        <v>4655</v>
       </c>
       <c r="P21" s="1">
-        <v>16095</v>
+        <v>14096</v>
       </c>
       <c r="Q21" s="1">
-        <v>646</v>
+        <v>40</v>
       </c>
       <c r="R21" s="1">
-        <v>13883</v>
+        <v>13730</v>
       </c>
       <c r="S21" s="1">
-        <v>3891</v>
+        <v>6697</v>
       </c>
       <c r="T21" s="1">
-        <v>7352</v>
+        <v>10976</v>
       </c>
       <c r="U21" s="1">
-        <v>5018</v>
+        <v>1989</v>
       </c>
       <c r="V21" s="1">
-        <v>4050</v>
+        <v>7396</v>
       </c>
     </row>
     <row r="22" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A22" s="1">
-        <v>2014</v>
+        <v>2013</v>
       </c>
       <c r="B22" s="1">
-        <v>29396</v>
+        <v>10583</v>
       </c>
       <c r="C22" s="1">
-        <v>7483</v>
+        <v>2297</v>
       </c>
       <c r="D22" s="1">
-        <v>44323</v>
+        <v>7848</v>
       </c>
       <c r="E22" s="1">
-        <v>47492</v>
+        <v>26946</v>
       </c>
       <c r="F22" s="1">
-        <v>1165</v>
+        <v>2207</v>
       </c>
       <c r="G22" s="1">
-        <v>42114</v>
+        <v>8883</v>
       </c>
       <c r="H22" s="1">
-        <v>15890</v>
+        <v>4870</v>
       </c>
       <c r="I22" s="1">
-        <v>6529</v>
+        <v>910</v>
       </c>
       <c r="J22" s="1">
-        <v>34858</v>
+        <v>5174</v>
       </c>
       <c r="K22" s="1">
-        <v>7261</v>
+        <v>1078</v>
       </c>
       <c r="L22" s="1">
-        <v>4536</v>
+        <v>3162</v>
       </c>
       <c r="M22" s="1">
-        <v>4195</v>
+        <v>1328</v>
       </c>
       <c r="N22" s="1">
-        <v>22225</v>
+        <v>8732</v>
       </c>
       <c r="O22" s="1">
-        <v>8183</v>
+        <v>4329</v>
       </c>
       <c r="P22" s="1">
-        <v>44341</v>
+        <v>16095</v>
       </c>
       <c r="Q22" s="1">
-        <v>467</v>
+        <v>646</v>
       </c>
       <c r="R22" s="1">
-        <v>13010</v>
+        <v>13883</v>
       </c>
       <c r="S22" s="1">
-        <v>4208</v>
+        <v>3891</v>
       </c>
       <c r="T22" s="1">
-        <v>12701</v>
+        <v>7352</v>
       </c>
       <c r="U22" s="1">
-        <v>22903</v>
+        <v>5018</v>
       </c>
       <c r="V22" s="1">
-        <v>29163</v>
+        <v>4050</v>
       </c>
     </row>
     <row r="23" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A23" s="1">
-        <v>2015</v>
+        <v>2014</v>
       </c>
       <c r="B23" s="1">
-        <v>7399</v>
+        <v>29396</v>
       </c>
       <c r="C23" s="1">
-        <v>398</v>
+        <v>7483</v>
       </c>
       <c r="D23" s="1">
-        <v>3636</v>
+        <v>44323</v>
       </c>
       <c r="E23" s="1">
-        <v>4028</v>
+        <v>47492</v>
       </c>
       <c r="F23" s="1">
-        <v>1902</v>
+        <v>1165</v>
       </c>
       <c r="G23" s="1">
-        <v>4470</v>
+        <v>42114</v>
       </c>
       <c r="H23" s="1">
-        <v>2694</v>
+        <v>15890</v>
       </c>
       <c r="I23" s="1">
-        <v>1016</v>
+        <v>6529</v>
       </c>
       <c r="J23" s="1">
-        <v>3695</v>
+        <v>34858</v>
       </c>
       <c r="K23" s="1">
-        <v>1235</v>
+        <v>7261</v>
       </c>
       <c r="L23" s="1">
-        <v>3594</v>
+        <v>4536</v>
       </c>
       <c r="M23" s="1">
-        <v>398</v>
+        <v>4195</v>
       </c>
       <c r="N23" s="1">
-        <v>2659</v>
+        <v>22225</v>
       </c>
       <c r="O23" s="1">
-        <v>1870</v>
+        <v>8183</v>
       </c>
       <c r="P23" s="1">
-        <v>12422</v>
+        <v>44341</v>
       </c>
       <c r="Q23" s="1">
-        <v>202</v>
+        <v>467</v>
       </c>
       <c r="R23" s="1">
-        <v>7054</v>
+        <v>13010</v>
       </c>
       <c r="S23" s="1">
-        <v>1302</v>
+        <v>4208</v>
       </c>
       <c r="T23" s="1">
-        <v>2503</v>
+        <v>12701</v>
       </c>
       <c r="U23" s="1">
-        <v>1614</v>
+        <v>22903</v>
       </c>
       <c r="V23" s="1">
-        <v>2880</v>
+        <v>29163</v>
       </c>
     </row>
     <row r="24" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A24" s="1">
-        <v>2016</v>
+        <v>2015</v>
       </c>
       <c r="B24" s="1">
-        <v>8039</v>
+        <v>7399</v>
       </c>
       <c r="C24" s="1">
-        <v>1863</v>
+        <v>398</v>
       </c>
       <c r="D24" s="1">
-        <v>5040</v>
+        <v>3636</v>
       </c>
       <c r="E24" s="1">
-        <v>10348</v>
+        <v>4028</v>
       </c>
       <c r="F24" s="1">
-        <v>1027</v>
+        <v>1902</v>
       </c>
       <c r="G24" s="1">
-        <v>4820</v>
+        <v>4470</v>
       </c>
       <c r="H24" s="1">
-        <v>1263</v>
+        <v>2694</v>
       </c>
       <c r="I24" s="1">
-        <v>1020</v>
+        <v>1016</v>
       </c>
       <c r="J24" s="1">
-        <v>8228</v>
+        <v>3695</v>
       </c>
       <c r="K24" s="1">
-        <v>2629</v>
+        <v>1235</v>
       </c>
       <c r="L24" s="1">
-        <v>1251</v>
+        <v>3594</v>
       </c>
       <c r="M24" s="1">
-        <v>1149</v>
+        <v>398</v>
       </c>
       <c r="N24" s="1">
-        <v>3286</v>
+        <v>2659</v>
       </c>
       <c r="O24" s="1">
-        <v>2639</v>
+        <v>1870</v>
       </c>
       <c r="P24" s="1">
-        <v>9964</v>
+        <v>12422</v>
       </c>
       <c r="Q24" s="1">
-        <v>131</v>
+        <v>202</v>
       </c>
       <c r="R24" s="1">
-        <v>834</v>
+        <v>7054</v>
       </c>
       <c r="S24" s="1">
-        <v>4768</v>
+        <v>1302</v>
       </c>
       <c r="T24" s="1">
-        <v>1361</v>
+        <v>2503</v>
       </c>
       <c r="U24" s="1">
-        <v>7741</v>
+        <v>1614</v>
       </c>
       <c r="V24" s="1">
-        <v>4066</v>
+        <v>2880</v>
       </c>
     </row>
     <row r="25" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A25" s="1">
-        <v>2017</v>
+        <v>2016</v>
       </c>
       <c r="B25" s="1">
-        <v>4931</v>
+        <v>8039</v>
       </c>
       <c r="C25" s="1">
-        <v>1786</v>
+        <v>1863</v>
       </c>
       <c r="D25" s="1">
-        <v>3092</v>
+        <v>5040</v>
       </c>
       <c r="E25" s="1">
-        <v>5337</v>
+        <v>10348</v>
       </c>
       <c r="F25" s="1">
-        <v>797</v>
+        <v>1027</v>
       </c>
       <c r="G25" s="1">
-        <v>12475</v>
+        <v>4820</v>
       </c>
       <c r="H25" s="1">
-        <v>2056</v>
+        <v>1263</v>
       </c>
       <c r="I25" s="1">
-        <v>608</v>
+        <v>1020</v>
       </c>
       <c r="J25" s="1">
-        <v>6309</v>
+        <v>8228</v>
       </c>
       <c r="K25" s="1">
-        <v>5169</v>
+        <v>2629</v>
       </c>
       <c r="L25" s="1">
-        <v>2038</v>
+        <v>1251</v>
       </c>
       <c r="M25" s="1">
-        <v>518</v>
+        <v>1149</v>
       </c>
       <c r="N25" s="1">
-        <v>5982</v>
+        <v>3286</v>
       </c>
       <c r="O25" s="1">
-        <v>822</v>
+        <v>2639</v>
       </c>
       <c r="P25" s="1">
-        <v>8198</v>
+        <v>9964</v>
       </c>
       <c r="Q25" s="1">
-        <v>79</v>
+        <v>131</v>
       </c>
       <c r="R25" s="1">
-        <v>1247</v>
+        <v>834</v>
       </c>
       <c r="S25" s="1">
-        <v>309</v>
+        <v>4768</v>
       </c>
       <c r="T25" s="1">
-        <v>366</v>
+        <v>1361</v>
       </c>
       <c r="U25" s="1">
-        <v>3366</v>
+        <v>7741</v>
       </c>
       <c r="V25" s="1">
-        <v>2865</v>
+        <v>4066</v>
       </c>
     </row>
     <row r="26" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A26" s="1">
-        <v>2018</v>
+        <v>2017</v>
       </c>
       <c r="B26" s="1">
-        <v>5720</v>
+        <v>4931</v>
       </c>
       <c r="C26" s="1">
-        <v>558</v>
+        <v>1786</v>
       </c>
       <c r="D26" s="1">
-        <v>8240</v>
+        <v>3092</v>
       </c>
       <c r="E26" s="1">
-        <v>6427</v>
+        <v>5337</v>
       </c>
       <c r="F26" s="1">
-        <v>710</v>
+        <v>797</v>
       </c>
       <c r="G26" s="1">
-        <v>15910</v>
+        <v>12475</v>
       </c>
       <c r="H26" s="1">
-        <v>4393</v>
+        <v>2056</v>
       </c>
       <c r="I26" s="1">
-        <v>444</v>
+        <v>608</v>
       </c>
       <c r="J26" s="1">
-        <v>4735</v>
+        <v>6309</v>
       </c>
       <c r="K26" s="1">
-        <v>1211</v>
+        <v>5169</v>
       </c>
       <c r="L26" s="1">
-        <v>3324</v>
+        <v>2038</v>
       </c>
       <c r="M26" s="1">
-        <v>116</v>
+        <v>518</v>
       </c>
       <c r="N26" s="1">
-        <v>4592</v>
+        <v>5982</v>
       </c>
       <c r="O26" s="1">
-        <v>2549</v>
+        <v>822</v>
       </c>
       <c r="P26" s="1">
-        <v>7498</v>
+        <v>8198</v>
       </c>
       <c r="Q26" s="1">
-        <v>197</v>
+        <v>79</v>
       </c>
       <c r="R26" s="1">
-        <v>3531</v>
+        <v>1247</v>
       </c>
       <c r="S26" s="1">
-        <v>1939</v>
+        <v>309</v>
       </c>
       <c r="T26" s="1">
-        <v>3130</v>
+        <v>366</v>
       </c>
       <c r="U26" s="1">
-        <v>2300</v>
+        <v>3366</v>
       </c>
       <c r="V26" s="1">
-        <v>5279</v>
+        <v>2865</v>
       </c>
     </row>
     <row r="27" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A27" s="1">
-        <v>2019</v>
+        <v>2018</v>
       </c>
       <c r="B27" s="1">
-        <v>5432</v>
+        <v>5720</v>
       </c>
       <c r="C27" s="1">
-        <v>912</v>
+        <v>558</v>
       </c>
       <c r="D27" s="1">
-        <v>14884</v>
+        <v>8240</v>
       </c>
       <c r="E27" s="1">
-        <v>13262</v>
+        <v>6427</v>
       </c>
       <c r="F27" s="1">
-        <v>1012</v>
+        <v>710</v>
       </c>
       <c r="G27" s="1">
-        <v>10250</v>
+        <v>15910</v>
       </c>
       <c r="H27" s="1">
-        <v>3476</v>
+        <v>4393</v>
       </c>
       <c r="I27" s="1">
-        <v>782</v>
+        <v>444</v>
       </c>
       <c r="J27" s="1">
-        <v>13869</v>
+        <v>4735</v>
       </c>
       <c r="K27" s="1">
-        <v>5154</v>
+        <v>1211</v>
       </c>
       <c r="L27" s="1">
-        <v>3698</v>
+        <v>3324</v>
       </c>
       <c r="M27" s="1">
-        <v>241</v>
+        <v>116</v>
       </c>
       <c r="N27" s="1">
-        <v>5050</v>
+        <v>4592</v>
       </c>
       <c r="O27" s="1">
-        <v>1193</v>
+        <v>2549</v>
       </c>
       <c r="P27" s="1">
-        <v>6587</v>
+        <v>7498</v>
       </c>
       <c r="Q27" s="1">
-        <v>174</v>
+        <v>197</v>
       </c>
       <c r="R27" s="1">
-        <v>4032</v>
+        <v>3531</v>
       </c>
       <c r="S27" s="1">
-        <v>1574</v>
+        <v>1939</v>
       </c>
       <c r="T27" s="1">
-        <v>5559</v>
+        <v>3130</v>
       </c>
       <c r="U27" s="1">
-        <v>4436</v>
+        <v>2300</v>
       </c>
       <c r="V27" s="1">
-        <v>3866</v>
+        <v>5279</v>
       </c>
     </row>
     <row r="28" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A28" s="1">
-        <v>2016</v>
+        <v>2019</v>
       </c>
       <c r="B28" s="1">
-        <v>8039</v>
+        <v>5432</v>
       </c>
       <c r="C28" s="1">
-        <v>1863</v>
+        <v>912</v>
       </c>
       <c r="D28" s="1">
-        <v>5040</v>
+        <v>14884</v>
       </c>
       <c r="E28" s="1">
-        <v>10348</v>
+        <v>13262</v>
       </c>
       <c r="F28" s="1">
-        <v>1027</v>
+        <v>1012</v>
       </c>
       <c r="G28" s="1">
-        <v>4820</v>
+        <v>10250</v>
       </c>
       <c r="H28" s="1">
-        <v>1263</v>
+        <v>3476</v>
       </c>
       <c r="I28" s="1">
-        <v>1020</v>
+        <v>782</v>
       </c>
       <c r="J28" s="1">
-        <v>8228</v>
+        <v>13869</v>
       </c>
       <c r="K28" s="1">
-        <v>2629</v>
+        <v>5154</v>
       </c>
       <c r="L28" s="1">
-        <v>1251</v>
+        <v>3698</v>
       </c>
       <c r="M28" s="1">
-        <v>1149</v>
+        <v>241</v>
       </c>
       <c r="N28" s="1">
-        <v>3286</v>
+        <v>5050</v>
       </c>
       <c r="O28" s="1">
-        <v>2639</v>
+        <v>1193</v>
       </c>
       <c r="P28" s="1">
-        <v>9964</v>
+        <v>6587</v>
       </c>
       <c r="Q28" s="1">
-        <v>131</v>
+        <v>174</v>
       </c>
       <c r="R28" s="1">
-        <v>834</v>
+        <v>4032</v>
       </c>
       <c r="S28" s="1">
-        <v>4768</v>
+        <v>1574</v>
       </c>
       <c r="T28" s="1">
-        <v>1361</v>
+        <v>5559</v>
       </c>
       <c r="U28" s="1">
-        <v>7741</v>
+        <v>4436</v>
       </c>
       <c r="V28" s="1">
-        <v>4066</v>
+        <v>3866</v>
       </c>
     </row>
     <row r="29" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A29" s="1">
-        <v>2017</v>
+        <v>2016</v>
       </c>
       <c r="B29" s="1">
-        <v>4931</v>
+        <v>8039</v>
       </c>
       <c r="C29" s="1">
-        <v>1786</v>
+        <v>1863</v>
       </c>
       <c r="D29" s="1">
-        <v>3092</v>
+        <v>5040</v>
       </c>
       <c r="E29" s="1">
-        <v>5337</v>
+        <v>10348</v>
       </c>
       <c r="F29" s="1">
-        <v>797</v>
+        <v>1027</v>
       </c>
       <c r="G29" s="1">
-        <v>12475</v>
+        <v>4820</v>
       </c>
       <c r="H29" s="1">
-        <v>2056</v>
+        <v>1263</v>
       </c>
       <c r="I29" s="1">
-        <v>608</v>
+        <v>1020</v>
       </c>
       <c r="J29" s="1">
-        <v>6309</v>
+        <v>8228</v>
       </c>
       <c r="K29" s="1">
-        <v>5169</v>
+        <v>2629</v>
       </c>
       <c r="L29" s="1">
-        <v>2038</v>
+        <v>1251</v>
       </c>
       <c r="M29" s="1">
-        <v>518</v>
+        <v>1149</v>
       </c>
       <c r="N29" s="1">
-        <v>5982</v>
+        <v>3286</v>
       </c>
       <c r="O29" s="1">
-        <v>822</v>
+        <v>2639</v>
       </c>
       <c r="P29" s="1">
-        <v>8198</v>
+        <v>9964</v>
       </c>
       <c r="Q29" s="1">
-        <v>79</v>
+        <v>131</v>
       </c>
       <c r="R29" s="1">
-        <v>1247</v>
+        <v>834</v>
       </c>
       <c r="S29" s="1">
-        <v>309</v>
+        <v>4768</v>
       </c>
       <c r="T29" s="1">
-        <v>366</v>
+        <v>1361</v>
       </c>
       <c r="U29" s="1">
-        <v>3366</v>
+        <v>7741</v>
       </c>
       <c r="V29" s="1">
-        <v>2865</v>
+        <v>4066</v>
       </c>
     </row>
     <row r="30" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A30" s="1">
-        <v>2018</v>
+        <v>2017</v>
       </c>
       <c r="B30" s="1">
-        <v>5720</v>
+        <v>4931</v>
       </c>
       <c r="C30" s="1">
-        <v>558</v>
+        <v>1786</v>
       </c>
       <c r="D30" s="1">
-        <v>8240</v>
+        <v>3092</v>
       </c>
       <c r="E30" s="1">
-        <v>6427</v>
+        <v>5337</v>
       </c>
       <c r="F30" s="1">
-        <v>710</v>
+        <v>797</v>
       </c>
       <c r="G30" s="1">
-        <v>15910</v>
+        <v>12475</v>
       </c>
       <c r="H30" s="1">
-        <v>4393</v>
+        <v>2056</v>
       </c>
       <c r="I30" s="1">
-        <v>444</v>
+        <v>608</v>
       </c>
       <c r="J30" s="1">
-        <v>4735</v>
+        <v>6309</v>
       </c>
       <c r="K30" s="1">
-        <v>1211</v>
+        <v>5169</v>
       </c>
       <c r="L30" s="1">
-        <v>3324</v>
+        <v>2038</v>
       </c>
       <c r="M30" s="1">
-        <v>116</v>
+        <v>518</v>
       </c>
       <c r="N30" s="1">
-        <v>4592</v>
+        <v>5982</v>
       </c>
       <c r="O30" s="1">
-        <v>2549</v>
+        <v>822</v>
       </c>
       <c r="P30" s="1">
-        <v>7498</v>
+        <v>8198</v>
       </c>
       <c r="Q30" s="1">
-        <v>197</v>
+        <v>79</v>
       </c>
       <c r="R30" s="1">
-        <v>3531</v>
+        <v>1247</v>
       </c>
       <c r="S30" s="1">
-        <v>1939</v>
+        <v>309</v>
       </c>
       <c r="T30" s="1">
-        <v>3130</v>
+        <v>366</v>
       </c>
       <c r="U30" s="1">
-        <v>2300</v>
+        <v>3366</v>
       </c>
       <c r="V30" s="1">
-        <v>5279</v>
+        <v>2865</v>
       </c>
     </row>
     <row r="31" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A31" s="1">
+        <v>2018</v>
+      </c>
+      <c r="B31" s="1">
+        <v>5720</v>
+      </c>
+      <c r="C31" s="1">
+        <v>558</v>
+      </c>
+      <c r="D31" s="1">
+        <v>8240</v>
+      </c>
+      <c r="E31" s="1">
+        <v>6427</v>
+      </c>
+      <c r="F31" s="1">
+        <v>710</v>
+      </c>
+      <c r="G31" s="1">
+        <v>15910</v>
+      </c>
+      <c r="H31" s="1">
+        <v>4393</v>
+      </c>
+      <c r="I31" s="1">
+        <v>444</v>
+      </c>
+      <c r="J31" s="1">
+        <v>4735</v>
+      </c>
+      <c r="K31" s="1">
+        <v>1211</v>
+      </c>
+      <c r="L31" s="1">
+        <v>3324</v>
+      </c>
+      <c r="M31" s="1">
+        <v>116</v>
+      </c>
+      <c r="N31" s="1">
+        <v>4592</v>
+      </c>
+      <c r="O31" s="1">
+        <v>2549</v>
+      </c>
+      <c r="P31" s="1">
+        <v>7498</v>
+      </c>
+      <c r="Q31" s="1">
+        <v>197</v>
+      </c>
+      <c r="R31" s="1">
+        <v>3531</v>
+      </c>
+      <c r="S31" s="1">
+        <v>1939</v>
+      </c>
+      <c r="T31" s="1">
+        <v>3130</v>
+      </c>
+      <c r="U31" s="1">
+        <v>2300</v>
+      </c>
+      <c r="V31" s="1">
+        <v>5279</v>
+      </c>
+    </row>
+    <row r="32" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A32" s="1">
         <v>2019</v>
       </c>
-      <c r="B31" s="1">
+      <c r="B32" s="1">
         <v>5432</v>
       </c>
-      <c r="C31" s="1">
+      <c r="C32" s="1">
         <v>912</v>
       </c>
-      <c r="D31" s="1">
+      <c r="D32" s="1">
         <v>14884</v>
       </c>
-      <c r="E31" s="1">
+      <c r="E32" s="1">
         <v>13262</v>
       </c>
-      <c r="F31" s="1">
+      <c r="F32" s="1">
         <v>1012</v>
       </c>
-      <c r="G31" s="1">
+      <c r="G32" s="1">
         <v>10250</v>
       </c>
-      <c r="H31" s="1">
+      <c r="H32" s="1">
         <v>3476</v>
       </c>
-      <c r="I31" s="1">
+      <c r="I32" s="1">
         <v>782</v>
       </c>
-      <c r="J31" s="1">
+      <c r="J32" s="1">
         <v>13869</v>
       </c>
-      <c r="K31" s="1">
+      <c r="K32" s="1">
         <v>5154</v>
       </c>
-      <c r="L31" s="1">
+      <c r="L32" s="1">
         <v>3698</v>
       </c>
-      <c r="M31" s="1">
+      <c r="M32" s="1">
         <v>241</v>
       </c>
-      <c r="N31" s="1">
+      <c r="N32" s="1">
         <v>5050</v>
       </c>
-      <c r="O31" s="1">
+      <c r="O32" s="1">
         <v>1193</v>
       </c>
-      <c r="P31" s="1">
+      <c r="P32" s="1">
         <v>6587</v>
       </c>
-      <c r="Q31" s="1">
+      <c r="Q32" s="1">
         <v>174</v>
       </c>
-      <c r="R31" s="1">
+      <c r="R32" s="1">
         <v>4032</v>
       </c>
-      <c r="S31" s="1">
+      <c r="S32" s="1">
         <v>1574</v>
       </c>
-      <c r="T31" s="1">
+      <c r="T32" s="1">
         <v>5559</v>
       </c>
-      <c r="U31" s="1">
+      <c r="U32" s="1">
         <v>4436</v>
       </c>
-      <c r="V31" s="1">
+      <c r="V32" s="1">
         <v>3866</v>
       </c>
     </row>
@@ -3147,7 +3155,7 @@
   <dimension ref="A1:X28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="S19" sqref="S19"/>
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Created some initial timeseries plots of salmon abundance by population. Removed the header in the data.
</commit_message>
<xml_diff>
--- a/data/OC Coho Abundance.xlsx
+++ b/data/OC Coho Abundance.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/oliviasomhegyi/Desktop/Grad School/GP/SalmonStocks/github/salmon_sisters/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7D69F78-547B-914B-B46D-093730D4670C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76E7BFDB-70A2-DC47-8C3B-4B70AC669544}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="27">
   <si>
     <t>Year</t>
   </si>
@@ -116,9 +116,6 @@
   </si>
   <si>
     <t>WILD COHO HARVEST ESTIMATES</t>
-  </si>
-  <si>
-    <t>TOTAL WILD ABUNDANCE</t>
   </si>
 </sst>
 </file>
@@ -1011,10 +1008,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:V32"/>
+  <dimension ref="A1:V31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1033,2115 +1030,2110 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A1" s="2" t="s">
-        <v>27</v>
+      <c r="A1" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="P1" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q1" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="R1" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="S1" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="T1" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="U1" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="V1" s="7" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="2" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A2" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="D2" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="E2" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="F2" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="G2" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="H2" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="I2" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="J2" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="K2" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="L2" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="M2" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="N2" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="O2" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="P2" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="Q2" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="R2" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="S2" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="T2" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="U2" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="V2" s="7" t="s">
-        <v>21</v>
+      <c r="A2" s="1">
+        <v>1994</v>
+      </c>
+      <c r="B2" s="1">
+        <v>878</v>
+      </c>
+      <c r="C2" s="1">
+        <v>716</v>
+      </c>
+      <c r="D2" s="1">
+        <v>15370</v>
+      </c>
+      <c r="E2" s="1">
+        <v>5426</v>
+      </c>
+      <c r="F2" s="1">
+        <v>2812</v>
+      </c>
+      <c r="G2" s="1">
+        <v>2928</v>
+      </c>
+      <c r="H2" s="1">
+        <v>2292</v>
+      </c>
+      <c r="I2" s="1">
+        <v>285</v>
+      </c>
+      <c r="J2" s="1">
+        <v>3015</v>
+      </c>
+      <c r="K2" s="1">
+        <v>282</v>
+      </c>
+      <c r="L2" s="1">
+        <v>953</v>
+      </c>
+      <c r="M2" s="1">
+        <v>96</v>
+      </c>
+      <c r="N2" s="1">
+        <v>658</v>
+      </c>
+      <c r="O2" s="1">
+        <v>1380</v>
+      </c>
+      <c r="P2" s="1">
+        <v>3349</v>
+      </c>
+      <c r="Q2" s="1">
+        <v>252</v>
+      </c>
+      <c r="R2" s="1">
+        <v>1146</v>
+      </c>
+      <c r="S2" s="1">
+        <v>1119</v>
+      </c>
+      <c r="T2" s="1">
+        <v>3555</v>
+      </c>
+      <c r="U2" s="1">
+        <v>1171</v>
+      </c>
+      <c r="V2" s="1">
+        <v>2162</v>
       </c>
     </row>
     <row r="3" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
-        <v>1994</v>
+        <v>1995</v>
       </c>
       <c r="B3" s="1">
-        <v>878</v>
+        <v>490</v>
       </c>
       <c r="C3" s="1">
-        <v>716</v>
+        <v>342</v>
       </c>
       <c r="D3" s="1">
-        <v>15370</v>
+        <v>11435</v>
       </c>
       <c r="E3" s="1">
-        <v>5426</v>
+        <v>2258</v>
       </c>
       <c r="F3" s="1">
-        <v>2812</v>
+        <v>1500</v>
       </c>
       <c r="G3" s="1">
-        <v>2928</v>
+        <v>12048</v>
       </c>
       <c r="H3" s="1">
-        <v>2292</v>
+        <v>3608</v>
       </c>
       <c r="I3" s="1">
-        <v>285</v>
+        <v>201</v>
       </c>
       <c r="J3" s="1">
-        <v>3015</v>
+        <v>1887</v>
       </c>
       <c r="K3" s="1">
-        <v>282</v>
+        <v>1706</v>
       </c>
       <c r="L3" s="1">
-        <v>953</v>
+        <v>1435</v>
       </c>
       <c r="M3" s="1">
-        <v>96</v>
+        <v>117</v>
       </c>
       <c r="N3" s="1">
-        <v>658</v>
+        <v>349</v>
       </c>
       <c r="O3" s="1">
-        <v>1380</v>
+        <v>4901</v>
       </c>
       <c r="P3" s="1">
-        <v>3349</v>
+        <v>6839</v>
       </c>
       <c r="Q3" s="1">
-        <v>252</v>
+        <v>85</v>
       </c>
       <c r="R3" s="1">
-        <v>1146</v>
+        <v>5234</v>
       </c>
       <c r="S3" s="1">
-        <v>1119</v>
+        <v>1750</v>
       </c>
       <c r="T3" s="1">
-        <v>3555</v>
+        <v>5652</v>
       </c>
       <c r="U3" s="1">
-        <v>1171</v>
+        <v>379</v>
       </c>
       <c r="V3" s="1">
-        <v>2162</v>
+        <v>5243</v>
       </c>
     </row>
     <row r="4" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
-        <v>1995</v>
+        <v>1996</v>
       </c>
       <c r="B4" s="1">
-        <v>490</v>
+        <v>1124</v>
       </c>
       <c r="C4" s="1">
-        <v>342</v>
+        <v>1374</v>
       </c>
       <c r="D4" s="1">
-        <v>11435</v>
+        <v>12856</v>
       </c>
       <c r="E4" s="1">
-        <v>2258</v>
+        <v>16763</v>
       </c>
       <c r="F4" s="1">
-        <v>1500</v>
+        <v>1610</v>
       </c>
       <c r="G4" s="1">
-        <v>12048</v>
+        <v>8464</v>
       </c>
       <c r="H4" s="1">
-        <v>3608</v>
+        <v>5391</v>
       </c>
       <c r="I4" s="1">
-        <v>201</v>
+        <v>441</v>
       </c>
       <c r="J4" s="1">
-        <v>1887</v>
+        <v>559</v>
       </c>
       <c r="K4" s="1">
-        <v>1706</v>
+        <v>466</v>
       </c>
       <c r="L4" s="1">
-        <v>1435</v>
+        <v>1133</v>
       </c>
       <c r="M4" s="1">
-        <v>117</v>
+        <v>87</v>
       </c>
       <c r="N4" s="1">
-        <v>349</v>
+        <v>419</v>
       </c>
       <c r="O4" s="1">
-        <v>4901</v>
+        <v>4989</v>
       </c>
       <c r="P4" s="1">
-        <v>6839</v>
+        <v>7668</v>
       </c>
       <c r="Q4" s="1">
-        <v>85</v>
+        <v>206</v>
       </c>
       <c r="R4" s="1">
-        <v>5234</v>
+        <v>7462</v>
       </c>
       <c r="S4" s="1">
-        <v>1750</v>
+        <v>1725</v>
       </c>
       <c r="T4" s="1">
-        <v>5652</v>
+        <v>7518</v>
       </c>
       <c r="U4" s="1">
-        <v>379</v>
+        <v>777</v>
       </c>
       <c r="V4" s="1">
-        <v>5243</v>
+        <v>4853</v>
       </c>
     </row>
     <row r="5" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
-        <v>1996</v>
+        <v>1997</v>
       </c>
       <c r="B5" s="1">
-        <v>1124</v>
+        <v>655</v>
       </c>
       <c r="C5" s="1">
-        <v>1374</v>
+        <v>542</v>
       </c>
       <c r="D5" s="1">
-        <v>12856</v>
+        <v>1212</v>
       </c>
       <c r="E5" s="1">
-        <v>16763</v>
+        <v>6235</v>
       </c>
       <c r="F5" s="1">
-        <v>1610</v>
+        <v>525</v>
       </c>
       <c r="G5" s="1">
-        <v>8464</v>
+        <v>1370</v>
       </c>
       <c r="H5" s="1">
-        <v>5391</v>
+        <v>614</v>
       </c>
       <c r="I5" s="1">
-        <v>441</v>
+        <v>106</v>
       </c>
       <c r="J5" s="1">
-        <v>559</v>
+        <v>1294</v>
       </c>
       <c r="K5" s="1">
-        <v>466</v>
+        <v>251</v>
       </c>
       <c r="L5" s="1">
-        <v>1133</v>
+        <v>629</v>
       </c>
       <c r="M5" s="1">
-        <v>87</v>
+        <v>17</v>
       </c>
       <c r="N5" s="1">
-        <v>419</v>
+        <v>325</v>
       </c>
       <c r="O5" s="1">
-        <v>4989</v>
+        <v>2892</v>
       </c>
       <c r="P5" s="1">
-        <v>7668</v>
+        <v>546</v>
       </c>
       <c r="Q5" s="1">
-        <v>206</v>
+        <v>156</v>
       </c>
       <c r="R5" s="1">
-        <v>7462</v>
+        <v>1021</v>
       </c>
       <c r="S5" s="1">
-        <v>1725</v>
+        <v>2008</v>
       </c>
       <c r="T5" s="1">
-        <v>7518</v>
+        <v>4460</v>
       </c>
       <c r="U5" s="1">
-        <v>777</v>
+        <v>476</v>
       </c>
       <c r="V5" s="1">
-        <v>4853</v>
+        <v>457</v>
       </c>
     </row>
     <row r="6" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
-        <v>1997</v>
+        <v>1998</v>
       </c>
       <c r="B6" s="1">
-        <v>655</v>
+        <v>117</v>
       </c>
       <c r="C6" s="1">
-        <v>542</v>
+        <v>433</v>
       </c>
       <c r="D6" s="1">
-        <v>1212</v>
+        <v>3224</v>
       </c>
       <c r="E6" s="1">
-        <v>6235</v>
+        <v>2605</v>
       </c>
       <c r="F6" s="1">
-        <v>525</v>
+        <v>949</v>
       </c>
       <c r="G6" s="1">
-        <v>1370</v>
+        <v>4916</v>
       </c>
       <c r="H6" s="1">
-        <v>614</v>
+        <v>1358</v>
       </c>
       <c r="I6" s="1">
-        <v>106</v>
+        <v>621</v>
       </c>
       <c r="J6" s="1">
-        <v>1294</v>
+        <v>1302</v>
       </c>
       <c r="K6" s="1">
-        <v>251</v>
+        <v>218</v>
       </c>
       <c r="L6" s="1">
-        <v>629</v>
+        <v>826</v>
       </c>
       <c r="M6" s="1">
-        <v>17</v>
+        <v>93</v>
       </c>
       <c r="N6" s="1">
-        <v>325</v>
+        <v>341</v>
       </c>
       <c r="O6" s="1">
-        <v>2892</v>
+        <v>3372</v>
       </c>
       <c r="P6" s="1">
-        <v>546</v>
+        <v>1102</v>
       </c>
       <c r="Q6" s="1">
-        <v>156</v>
+        <v>603</v>
       </c>
       <c r="R6" s="1">
-        <v>1021</v>
+        <v>3431</v>
       </c>
       <c r="S6" s="1">
-        <v>2008</v>
+        <v>3042</v>
       </c>
       <c r="T6" s="1">
-        <v>4460</v>
+        <v>5583</v>
       </c>
       <c r="U6" s="1">
-        <v>476</v>
+        <v>387</v>
       </c>
       <c r="V6" s="1">
-        <v>457</v>
+        <v>551</v>
       </c>
     </row>
     <row r="7" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
-        <v>1998</v>
+        <v>1999</v>
       </c>
       <c r="B7" s="1">
-        <v>117</v>
+        <v>1435</v>
       </c>
       <c r="C7" s="1">
-        <v>433</v>
+        <v>1617</v>
       </c>
       <c r="D7" s="1">
-        <v>3224</v>
+        <v>5155</v>
       </c>
       <c r="E7" s="1">
-        <v>2605</v>
+        <v>2854</v>
       </c>
       <c r="F7" s="1">
-        <v>949</v>
+        <v>717</v>
       </c>
       <c r="G7" s="1">
-        <v>4916</v>
+        <v>2807</v>
       </c>
       <c r="H7" s="1">
-        <v>1358</v>
+        <v>1870</v>
       </c>
       <c r="I7" s="1">
-        <v>621</v>
+        <v>376</v>
       </c>
       <c r="J7" s="1">
-        <v>1302</v>
+        <v>3804</v>
       </c>
       <c r="K7" s="1">
-        <v>218</v>
+        <v>2522</v>
       </c>
       <c r="L7" s="1">
-        <v>826</v>
+        <v>1278</v>
       </c>
       <c r="M7" s="1">
-        <v>93</v>
+        <v>15</v>
       </c>
       <c r="N7" s="1">
-        <v>341</v>
+        <v>1294</v>
       </c>
       <c r="O7" s="1">
-        <v>3372</v>
+        <v>2949</v>
       </c>
       <c r="P7" s="1">
-        <v>1102</v>
+        <v>3189</v>
       </c>
       <c r="Q7" s="1">
-        <v>603</v>
+        <v>60</v>
       </c>
       <c r="R7" s="1">
-        <v>3431</v>
+        <v>3222</v>
       </c>
       <c r="S7" s="1">
-        <v>3042</v>
+        <v>3920</v>
       </c>
       <c r="T7" s="1">
-        <v>5583</v>
+        <v>6552</v>
       </c>
       <c r="U7" s="1">
-        <v>387</v>
+        <v>1959</v>
       </c>
       <c r="V7" s="1">
-        <v>551</v>
+        <v>2742</v>
       </c>
     </row>
     <row r="8" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
-        <v>1999</v>
+        <v>2000</v>
       </c>
       <c r="B8" s="1">
-        <v>1435</v>
+        <v>3498</v>
       </c>
       <c r="C8" s="1">
-        <v>1617</v>
+        <v>1523</v>
       </c>
       <c r="D8" s="1">
-        <v>5155</v>
+        <v>4892</v>
       </c>
       <c r="E8" s="1">
-        <v>2854</v>
+        <v>6503</v>
       </c>
       <c r="F8" s="1">
-        <v>717</v>
+        <v>1536</v>
       </c>
       <c r="G8" s="1">
-        <v>2807</v>
+        <v>6012</v>
       </c>
       <c r="H8" s="1">
-        <v>1870</v>
+        <v>4737</v>
       </c>
       <c r="I8" s="1">
-        <v>376</v>
+        <v>373</v>
       </c>
       <c r="J8" s="1">
-        <v>3804</v>
+        <v>15040</v>
       </c>
       <c r="K8" s="1">
-        <v>2522</v>
+        <v>1268</v>
       </c>
       <c r="L8" s="1">
-        <v>1278</v>
+        <v>1744</v>
       </c>
       <c r="M8" s="1">
-        <v>15</v>
+        <v>186</v>
       </c>
       <c r="N8" s="1">
-        <v>1294</v>
+        <v>3522</v>
       </c>
       <c r="O8" s="1">
-        <v>2949</v>
+        <v>3988</v>
       </c>
       <c r="P8" s="1">
-        <v>3189</v>
+        <v>6793</v>
       </c>
       <c r="Q8" s="1">
-        <v>60</v>
+        <v>141</v>
       </c>
       <c r="R8" s="1">
-        <v>3222</v>
+        <v>2684</v>
       </c>
       <c r="S8" s="1">
-        <v>3920</v>
+        <v>659</v>
       </c>
       <c r="T8" s="1">
-        <v>6552</v>
+        <v>8609</v>
       </c>
       <c r="U8" s="1">
-        <v>1959</v>
+        <v>2265</v>
       </c>
       <c r="V8" s="1">
-        <v>2742</v>
+        <v>662</v>
       </c>
     </row>
     <row r="9" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
-        <v>2000</v>
+        <v>2001</v>
       </c>
       <c r="B9" s="1">
-        <v>3498</v>
+        <v>3357</v>
       </c>
       <c r="C9" s="1">
-        <v>1523</v>
+        <v>1905</v>
       </c>
       <c r="D9" s="1">
-        <v>4892</v>
+        <v>34939</v>
       </c>
       <c r="E9" s="1">
-        <v>6503</v>
+        <v>14386</v>
       </c>
       <c r="F9" s="1">
-        <v>1536</v>
+        <v>5891</v>
       </c>
       <c r="G9" s="1">
-        <v>6012</v>
+        <v>12105</v>
       </c>
       <c r="H9" s="1">
-        <v>4737</v>
+        <v>9298</v>
       </c>
       <c r="I9" s="1">
-        <v>373</v>
+        <v>5025</v>
       </c>
       <c r="J9" s="1">
-        <v>15040</v>
+        <v>22805</v>
       </c>
       <c r="K9" s="1">
-        <v>1268</v>
+        <v>4331</v>
       </c>
       <c r="L9" s="1">
-        <v>1744</v>
+        <v>2739</v>
       </c>
       <c r="M9" s="1">
-        <v>186</v>
+        <v>234</v>
       </c>
       <c r="N9" s="1">
-        <v>3522</v>
+        <v>1659</v>
       </c>
       <c r="O9" s="1">
-        <v>3988</v>
+        <v>5308</v>
       </c>
       <c r="P9" s="1">
-        <v>6793</v>
+        <v>11030</v>
       </c>
       <c r="Q9" s="1">
-        <v>141</v>
+        <v>99</v>
       </c>
       <c r="R9" s="1">
-        <v>2684</v>
+        <v>12346</v>
       </c>
       <c r="S9" s="1">
-        <v>659</v>
+        <v>3650</v>
       </c>
       <c r="T9" s="1">
-        <v>8609</v>
+        <v>11430</v>
       </c>
       <c r="U9" s="1">
-        <v>2265</v>
+        <v>2022</v>
       </c>
       <c r="V9" s="1">
-        <v>662</v>
+        <v>3733</v>
       </c>
     </row>
     <row r="10" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
-        <v>2001</v>
+        <v>2002</v>
       </c>
       <c r="B10" s="1">
-        <v>3357</v>
+        <v>9527</v>
       </c>
       <c r="C10" s="1">
-        <v>1905</v>
+        <v>3378</v>
       </c>
       <c r="D10" s="1">
-        <v>34939</v>
+        <v>34776</v>
       </c>
       <c r="E10" s="1">
-        <v>14386</v>
+        <v>8060</v>
       </c>
       <c r="F10" s="1">
-        <v>5891</v>
+        <v>3436</v>
       </c>
       <c r="G10" s="1">
-        <v>12105</v>
+        <v>19825</v>
       </c>
       <c r="H10" s="1">
-        <v>9298</v>
+        <v>11275</v>
       </c>
       <c r="I10" s="1">
-        <v>5025</v>
+        <v>2149</v>
       </c>
       <c r="J10" s="1">
-        <v>22805</v>
+        <v>18022</v>
       </c>
       <c r="K10" s="1">
-        <v>4331</v>
+        <v>17533</v>
       </c>
       <c r="L10" s="1">
-        <v>2739</v>
+        <v>3536</v>
       </c>
       <c r="M10" s="1">
-        <v>234</v>
+        <v>570</v>
       </c>
       <c r="N10" s="1">
-        <v>1659</v>
+        <v>2235</v>
       </c>
       <c r="O10" s="1">
-        <v>5308</v>
+        <v>4868</v>
       </c>
       <c r="P10" s="1">
-        <v>11030</v>
+        <v>58217</v>
       </c>
       <c r="Q10" s="1">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="R10" s="1">
-        <v>12346</v>
+        <v>11043</v>
       </c>
       <c r="S10" s="1">
-        <v>3650</v>
+        <v>3654</v>
       </c>
       <c r="T10" s="1">
-        <v>11430</v>
+        <v>14554</v>
       </c>
       <c r="U10" s="1">
-        <v>2022</v>
+        <v>14001</v>
       </c>
       <c r="V10" s="1">
-        <v>3733</v>
+        <v>24990</v>
       </c>
     </row>
     <row r="11" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
-        <v>2002</v>
+        <v>2003</v>
       </c>
       <c r="B11" s="1">
-        <v>9527</v>
+        <v>11103</v>
       </c>
       <c r="C11" s="1">
-        <v>3378</v>
+        <v>5996</v>
       </c>
       <c r="D11" s="1">
-        <v>34776</v>
+        <v>27822</v>
       </c>
       <c r="E11" s="1">
-        <v>8060</v>
+        <v>24195</v>
       </c>
       <c r="F11" s="1">
-        <v>3436</v>
+        <v>1028</v>
       </c>
       <c r="G11" s="1">
-        <v>19825</v>
+        <v>17814</v>
       </c>
       <c r="H11" s="1">
-        <v>11275</v>
+        <v>11977</v>
       </c>
       <c r="I11" s="1">
-        <v>2149</v>
+        <v>2567</v>
       </c>
       <c r="J11" s="1">
-        <v>18022</v>
+        <v>35118</v>
       </c>
       <c r="K11" s="1">
-        <v>17533</v>
+        <v>11010</v>
       </c>
       <c r="L11" s="1">
-        <v>3536</v>
+        <v>3091</v>
       </c>
       <c r="M11" s="1">
-        <v>570</v>
+        <v>45</v>
       </c>
       <c r="N11" s="1">
-        <v>2235</v>
+        <v>8681</v>
       </c>
       <c r="O11" s="1">
-        <v>4868</v>
+        <v>7158</v>
       </c>
       <c r="P11" s="1">
-        <v>58217</v>
+        <v>31323</v>
       </c>
       <c r="Q11" s="1">
-        <v>100</v>
+        <v>93</v>
       </c>
       <c r="R11" s="1">
-        <v>11043</v>
+        <v>4684</v>
       </c>
       <c r="S11" s="1">
-        <v>3654</v>
+        <v>3443</v>
       </c>
       <c r="T11" s="1">
-        <v>14554</v>
+        <v>6761</v>
       </c>
       <c r="U11" s="1">
-        <v>14001</v>
+        <v>14049</v>
       </c>
       <c r="V11" s="1">
-        <v>24990</v>
+        <v>17803</v>
       </c>
     </row>
     <row r="12" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
-        <v>2003</v>
+        <v>2004</v>
       </c>
       <c r="B12" s="1">
-        <v>11103</v>
+        <v>5652</v>
       </c>
       <c r="C12" s="1">
-        <v>5996</v>
+        <v>4935</v>
       </c>
       <c r="D12" s="1">
-        <v>27822</v>
+        <v>25204</v>
       </c>
       <c r="E12" s="1">
-        <v>24195</v>
+        <v>23909</v>
       </c>
       <c r="F12" s="1">
-        <v>1028</v>
+        <v>8042</v>
       </c>
       <c r="G12" s="1">
-        <v>17814</v>
+        <v>9708</v>
       </c>
       <c r="H12" s="1">
-        <v>11977</v>
+        <v>6885</v>
       </c>
       <c r="I12" s="1">
-        <v>2567</v>
+        <v>2374</v>
       </c>
       <c r="J12" s="1">
-        <v>35118</v>
+        <v>20235</v>
       </c>
       <c r="K12" s="1">
-        <v>11010</v>
+        <v>5071</v>
       </c>
       <c r="L12" s="1">
-        <v>3091</v>
+        <v>3844</v>
       </c>
       <c r="M12" s="1">
-        <v>45</v>
+        <v>1773</v>
       </c>
       <c r="N12" s="1">
-        <v>8681</v>
+        <v>8833</v>
       </c>
       <c r="O12" s="1">
-        <v>7158</v>
+        <v>8638</v>
       </c>
       <c r="P12" s="1">
-        <v>31323</v>
+        <v>9427</v>
       </c>
       <c r="Q12" s="1">
-        <v>93</v>
+        <v>435</v>
       </c>
       <c r="R12" s="1">
-        <v>4684</v>
+        <v>11877</v>
       </c>
       <c r="S12" s="1">
-        <v>3443</v>
+        <v>3776</v>
       </c>
       <c r="T12" s="1">
-        <v>6761</v>
+        <v>7720</v>
       </c>
       <c r="U12" s="1">
-        <v>14049</v>
+        <v>2735</v>
       </c>
       <c r="V12" s="1">
-        <v>17803</v>
+        <v>5982</v>
       </c>
     </row>
     <row r="13" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A13" s="1">
-        <v>2004</v>
+        <v>2005</v>
       </c>
       <c r="B13" s="1">
-        <v>5652</v>
+        <v>14463</v>
       </c>
       <c r="C13" s="1">
-        <v>4935</v>
+        <v>2355</v>
       </c>
       <c r="D13" s="1">
-        <v>25204</v>
+        <v>17730</v>
       </c>
       <c r="E13" s="1">
-        <v>23909</v>
+        <v>12278</v>
       </c>
       <c r="F13" s="1">
-        <v>8042</v>
+        <v>526</v>
       </c>
       <c r="G13" s="1">
-        <v>9708</v>
+        <v>19335</v>
       </c>
       <c r="H13" s="1">
-        <v>6885</v>
+        <v>7912</v>
       </c>
       <c r="I13" s="1">
-        <v>2374</v>
+        <v>1267</v>
       </c>
       <c r="J13" s="1">
-        <v>20235</v>
+        <v>10869</v>
       </c>
       <c r="K13" s="1">
-        <v>5071</v>
+        <v>713</v>
       </c>
       <c r="L13" s="1">
-        <v>3844</v>
+        <v>2048</v>
       </c>
       <c r="M13" s="1">
-        <v>1773</v>
+        <v>82</v>
       </c>
       <c r="N13" s="1">
-        <v>8833</v>
+        <v>15150</v>
       </c>
       <c r="O13" s="1">
-        <v>8638</v>
+        <v>4539</v>
       </c>
       <c r="P13" s="1">
-        <v>9427</v>
+        <v>17583</v>
       </c>
       <c r="Q13" s="1">
-        <v>435</v>
+        <v>109</v>
       </c>
       <c r="R13" s="1">
-        <v>11877</v>
+        <v>14939</v>
       </c>
       <c r="S13" s="1">
-        <v>3776</v>
+        <v>1973</v>
       </c>
       <c r="T13" s="1">
-        <v>7720</v>
+        <v>8803</v>
       </c>
       <c r="U13" s="1">
-        <v>2735</v>
+        <v>2075</v>
       </c>
       <c r="V13" s="1">
-        <v>5982</v>
+        <v>3579</v>
       </c>
     </row>
     <row r="14" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A14" s="1">
-        <v>2005</v>
+        <v>2006</v>
       </c>
       <c r="B14" s="1">
-        <v>14463</v>
+        <v>2130</v>
       </c>
       <c r="C14" s="1">
-        <v>2355</v>
+        <v>2106</v>
       </c>
       <c r="D14" s="1">
-        <v>17730</v>
+        <v>12167</v>
       </c>
       <c r="E14" s="1">
-        <v>12278</v>
+        <v>30863</v>
       </c>
       <c r="F14" s="1">
-        <v>526</v>
+        <v>1192</v>
       </c>
       <c r="G14" s="1">
-        <v>19335</v>
+        <v>8634</v>
       </c>
       <c r="H14" s="1">
-        <v>7912</v>
+        <v>5240</v>
       </c>
       <c r="I14" s="1">
-        <v>1267</v>
+        <v>810</v>
       </c>
       <c r="J14" s="1">
-        <v>10869</v>
+        <v>12543</v>
       </c>
       <c r="K14" s="1">
-        <v>713</v>
+        <v>2026</v>
       </c>
       <c r="L14" s="1">
-        <v>2048</v>
+        <v>3240</v>
       </c>
       <c r="M14" s="1">
-        <v>82</v>
+        <v>554</v>
       </c>
       <c r="N14" s="1">
-        <v>15150</v>
+        <v>5621</v>
       </c>
       <c r="O14" s="1">
-        <v>4539</v>
+        <v>5888</v>
       </c>
       <c r="P14" s="1">
-        <v>17583</v>
+        <v>6339</v>
       </c>
       <c r="Q14" s="1">
-        <v>109</v>
+        <v>318</v>
       </c>
       <c r="R14" s="1">
-        <v>14939</v>
+        <v>2426</v>
       </c>
       <c r="S14" s="1">
-        <v>1973</v>
+        <v>3900</v>
       </c>
       <c r="T14" s="1">
-        <v>8803</v>
+        <v>16269</v>
       </c>
       <c r="U14" s="1">
-        <v>2075</v>
+        <v>9476</v>
       </c>
       <c r="V14" s="1">
-        <v>3579</v>
+        <v>4587</v>
       </c>
     </row>
     <row r="15" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A15" s="1">
-        <v>2006</v>
+        <v>2007</v>
       </c>
       <c r="B15" s="1">
-        <v>2130</v>
+        <v>2404</v>
       </c>
       <c r="C15" s="1">
-        <v>2106</v>
+        <v>684</v>
       </c>
       <c r="D15" s="1">
-        <v>12167</v>
+        <v>1488</v>
       </c>
       <c r="E15" s="1">
-        <v>30863</v>
+        <v>15644</v>
       </c>
       <c r="F15" s="1">
-        <v>1192</v>
+        <v>381</v>
       </c>
       <c r="G15" s="1">
-        <v>8634</v>
+        <v>4745</v>
       </c>
       <c r="H15" s="1">
-        <v>5240</v>
+        <v>1777</v>
       </c>
       <c r="I15" s="1">
-        <v>810</v>
+        <v>483</v>
       </c>
       <c r="J15" s="1">
-        <v>12543</v>
+        <v>15717</v>
       </c>
       <c r="K15" s="1">
-        <v>2026</v>
+        <v>441</v>
       </c>
       <c r="L15" s="1">
-        <v>3240</v>
+        <v>1579</v>
       </c>
       <c r="M15" s="1">
-        <v>554</v>
+        <v>66</v>
       </c>
       <c r="N15" s="1">
-        <v>5621</v>
+        <v>2461</v>
       </c>
       <c r="O15" s="1">
-        <v>5888</v>
+        <v>1621</v>
       </c>
       <c r="P15" s="1">
-        <v>6339</v>
+        <v>3978</v>
       </c>
       <c r="Q15" s="1">
-        <v>318</v>
+        <v>109</v>
       </c>
       <c r="R15" s="1">
-        <v>2426</v>
+        <v>5095</v>
       </c>
       <c r="S15" s="1">
-        <v>3900</v>
+        <v>3977</v>
       </c>
       <c r="T15" s="1">
-        <v>16269</v>
+        <v>4432</v>
       </c>
       <c r="U15" s="1">
-        <v>9476</v>
+        <v>2570</v>
       </c>
       <c r="V15" s="1">
-        <v>4587</v>
+        <v>3537</v>
       </c>
     </row>
     <row r="16" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A16" s="1">
-        <v>2007</v>
+        <v>2008</v>
       </c>
       <c r="B16" s="1">
-        <v>2404</v>
+        <v>13586</v>
       </c>
       <c r="C16" s="1">
-        <v>684</v>
+        <v>1242</v>
       </c>
       <c r="D16" s="1">
-        <v>1488</v>
+        <v>15179</v>
       </c>
       <c r="E16" s="1">
-        <v>15644</v>
+        <v>8967</v>
       </c>
       <c r="F16" s="1">
-        <v>381</v>
+        <v>802</v>
       </c>
       <c r="G16" s="1">
-        <v>4745</v>
+        <v>9203</v>
       </c>
       <c r="H16" s="1">
-        <v>1777</v>
+        <v>4561</v>
       </c>
       <c r="I16" s="1">
-        <v>483</v>
+        <v>1076</v>
       </c>
       <c r="J16" s="1">
-        <v>15717</v>
+        <v>17549</v>
       </c>
       <c r="K16" s="1">
-        <v>441</v>
+        <v>1881</v>
       </c>
       <c r="L16" s="1">
-        <v>1579</v>
+        <v>3507</v>
       </c>
       <c r="M16" s="1">
-        <v>66</v>
+        <v>665</v>
       </c>
       <c r="N16" s="1">
-        <v>2461</v>
+        <v>21047</v>
       </c>
       <c r="O16" s="1">
-        <v>1621</v>
+        <v>3950</v>
       </c>
       <c r="P16" s="1">
-        <v>3978</v>
+        <v>17841</v>
       </c>
       <c r="Q16" s="1">
-        <v>109</v>
+        <v>44</v>
       </c>
       <c r="R16" s="1">
-        <v>5095</v>
+        <v>21354</v>
       </c>
       <c r="S16" s="1">
-        <v>3977</v>
+        <v>2656</v>
       </c>
       <c r="T16" s="1">
-        <v>4432</v>
+        <v>17474</v>
       </c>
       <c r="U16" s="1">
-        <v>2570</v>
+        <v>4925</v>
       </c>
       <c r="V16" s="1">
-        <v>3537</v>
+        <v>11131</v>
       </c>
     </row>
     <row r="17" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A17" s="1">
-        <v>2008</v>
+        <v>2009</v>
       </c>
       <c r="B17" s="1">
-        <v>13586</v>
+        <v>15663</v>
       </c>
       <c r="C17" s="1">
-        <v>1242</v>
+        <v>3825</v>
       </c>
       <c r="D17" s="1">
-        <v>15179</v>
+        <v>28868</v>
       </c>
       <c r="E17" s="1">
-        <v>8967</v>
+        <v>23846</v>
       </c>
       <c r="F17" s="1">
-        <v>802</v>
+        <v>3427</v>
       </c>
       <c r="G17" s="1">
-        <v>9203</v>
+        <v>20592</v>
       </c>
       <c r="H17" s="1">
-        <v>4561</v>
+        <v>16130</v>
       </c>
       <c r="I17" s="1">
-        <v>1076</v>
+        <v>4095</v>
       </c>
       <c r="J17" s="1">
-        <v>17549</v>
+        <v>23276</v>
       </c>
       <c r="K17" s="1">
-        <v>1881</v>
+        <v>4550</v>
       </c>
       <c r="L17" s="1">
-        <v>3507</v>
+        <v>8260</v>
       </c>
       <c r="M17" s="1">
-        <v>665</v>
+        <v>806</v>
       </c>
       <c r="N17" s="1">
-        <v>21047</v>
+        <v>25755</v>
       </c>
       <c r="O17" s="1">
-        <v>3950</v>
+        <v>5561</v>
       </c>
       <c r="P17" s="1">
-        <v>17841</v>
+        <v>32749</v>
       </c>
       <c r="Q17" s="1">
-        <v>44</v>
+        <v>188</v>
       </c>
       <c r="R17" s="1">
-        <v>21354</v>
+        <v>17060</v>
       </c>
       <c r="S17" s="1">
-        <v>2656</v>
+        <v>3185</v>
       </c>
       <c r="T17" s="1">
-        <v>17474</v>
+        <v>9817</v>
       </c>
       <c r="U17" s="1">
-        <v>4925</v>
+        <v>17389</v>
       </c>
       <c r="V17" s="1">
-        <v>11131</v>
+        <v>11965</v>
       </c>
     </row>
     <row r="18" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A18" s="1">
-        <v>2009</v>
+        <v>2010</v>
       </c>
       <c r="B18" s="1">
-        <v>15663</v>
+        <v>10172</v>
       </c>
       <c r="C18" s="1">
-        <v>3825</v>
+        <v>2176</v>
       </c>
       <c r="D18" s="1">
-        <v>28868</v>
+        <v>29041</v>
       </c>
       <c r="E18" s="1">
-        <v>23846</v>
+        <v>24742</v>
       </c>
       <c r="F18" s="1">
-        <v>3427</v>
+        <v>11895</v>
       </c>
       <c r="G18" s="1">
-        <v>20592</v>
+        <v>18392</v>
       </c>
       <c r="H18" s="1">
-        <v>16130</v>
+        <v>19029</v>
       </c>
       <c r="I18" s="1">
-        <v>4095</v>
+        <v>4667</v>
       </c>
       <c r="J18" s="1">
-        <v>23276</v>
+        <v>33826</v>
       </c>
       <c r="K18" s="1">
-        <v>4550</v>
+        <v>2044</v>
       </c>
       <c r="L18" s="1">
-        <v>8260</v>
+        <v>9867</v>
       </c>
       <c r="M18" s="1">
-        <v>806</v>
+        <v>1451</v>
       </c>
       <c r="N18" s="1">
-        <v>25755</v>
+        <v>6597</v>
       </c>
       <c r="O18" s="1">
-        <v>5561</v>
+        <v>8062</v>
       </c>
       <c r="P18" s="1">
-        <v>32749</v>
+        <v>27282</v>
       </c>
       <c r="Q18" s="1">
-        <v>188</v>
+        <v>97</v>
       </c>
       <c r="R18" s="1">
-        <v>17060</v>
+        <v>26232</v>
       </c>
       <c r="S18" s="1">
-        <v>3185</v>
+        <v>11215</v>
       </c>
       <c r="T18" s="1">
-        <v>9817</v>
+        <v>21404</v>
       </c>
       <c r="U18" s="1">
-        <v>17389</v>
+        <v>15635</v>
       </c>
       <c r="V18" s="1">
-        <v>11965</v>
+        <v>9018</v>
       </c>
     </row>
     <row r="19" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A19" s="1">
-        <v>2010</v>
+        <v>2011</v>
       </c>
       <c r="B19" s="1">
-        <v>10172</v>
+        <v>30037</v>
       </c>
       <c r="C19" s="1">
-        <v>2176</v>
+        <v>2532</v>
       </c>
       <c r="D19" s="1">
-        <v>29041</v>
+        <v>11659</v>
       </c>
       <c r="E19" s="1">
-        <v>24742</v>
+        <v>59007</v>
       </c>
       <c r="F19" s="1">
-        <v>11895</v>
+        <v>9770</v>
       </c>
       <c r="G19" s="1">
-        <v>18392</v>
+        <v>19838</v>
       </c>
       <c r="H19" s="1">
-        <v>19029</v>
+        <v>21160</v>
       </c>
       <c r="I19" s="1">
-        <v>4667</v>
+        <v>2247</v>
       </c>
       <c r="J19" s="1">
-        <v>33826</v>
+        <v>16241</v>
       </c>
       <c r="K19" s="1">
-        <v>2044</v>
+        <v>8328</v>
       </c>
       <c r="L19" s="1">
-        <v>9867</v>
+        <v>6381</v>
       </c>
       <c r="M19" s="1">
-        <v>1451</v>
+        <v>3854</v>
       </c>
       <c r="N19" s="1">
-        <v>6597</v>
+        <v>35080</v>
       </c>
       <c r="O19" s="1">
-        <v>8062</v>
+        <v>6735</v>
       </c>
       <c r="P19" s="1">
-        <v>27282</v>
+        <v>29767</v>
       </c>
       <c r="Q19" s="1">
-        <v>97</v>
+        <v>354</v>
       </c>
       <c r="R19" s="1">
-        <v>26232</v>
+        <v>52955</v>
       </c>
       <c r="S19" s="1">
-        <v>11215</v>
+        <v>7043</v>
       </c>
       <c r="T19" s="1">
-        <v>21404</v>
+        <v>7721</v>
       </c>
       <c r="U19" s="1">
-        <v>15635</v>
+        <v>20405</v>
       </c>
       <c r="V19" s="1">
-        <v>9018</v>
+        <v>20218</v>
       </c>
     </row>
     <row r="20" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A20" s="1">
-        <v>2011</v>
+        <v>2012</v>
       </c>
       <c r="B20" s="1">
-        <v>30037</v>
+        <v>9995</v>
       </c>
       <c r="C20" s="1">
-        <v>2532</v>
+        <v>2216</v>
       </c>
       <c r="D20" s="1">
-        <v>11659</v>
+        <v>11109</v>
       </c>
       <c r="E20" s="1">
-        <v>59007</v>
+        <v>6975</v>
       </c>
       <c r="F20" s="1">
-        <v>9770</v>
+        <v>2952</v>
       </c>
       <c r="G20" s="1">
-        <v>19838</v>
+        <v>4403</v>
       </c>
       <c r="H20" s="1">
-        <v>21160</v>
+        <v>2887</v>
       </c>
       <c r="I20" s="1">
-        <v>2247</v>
+        <v>1064</v>
       </c>
       <c r="J20" s="1">
-        <v>16241</v>
+        <v>3496</v>
       </c>
       <c r="K20" s="1">
-        <v>8328</v>
+        <v>2066</v>
       </c>
       <c r="L20" s="1">
-        <v>6381</v>
+        <v>3698</v>
       </c>
       <c r="M20" s="1">
-        <v>3854</v>
+        <v>350</v>
       </c>
       <c r="N20" s="1">
-        <v>35080</v>
+        <v>5304</v>
       </c>
       <c r="O20" s="1">
-        <v>6735</v>
+        <v>4655</v>
       </c>
       <c r="P20" s="1">
-        <v>29767</v>
+        <v>14096</v>
       </c>
       <c r="Q20" s="1">
-        <v>354</v>
+        <v>40</v>
       </c>
       <c r="R20" s="1">
-        <v>52955</v>
+        <v>13730</v>
       </c>
       <c r="S20" s="1">
-        <v>7043</v>
+        <v>6697</v>
       </c>
       <c r="T20" s="1">
-        <v>7721</v>
+        <v>10976</v>
       </c>
       <c r="U20" s="1">
-        <v>20405</v>
+        <v>1989</v>
       </c>
       <c r="V20" s="1">
-        <v>20218</v>
+        <v>7396</v>
       </c>
     </row>
     <row r="21" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A21" s="1">
-        <v>2012</v>
+        <v>2013</v>
       </c>
       <c r="B21" s="1">
-        <v>9995</v>
+        <v>10583</v>
       </c>
       <c r="C21" s="1">
-        <v>2216</v>
+        <v>2297</v>
       </c>
       <c r="D21" s="1">
-        <v>11109</v>
+        <v>7848</v>
       </c>
       <c r="E21" s="1">
-        <v>6975</v>
+        <v>26946</v>
       </c>
       <c r="F21" s="1">
-        <v>2952</v>
+        <v>2207</v>
       </c>
       <c r="G21" s="1">
-        <v>4403</v>
+        <v>8883</v>
       </c>
       <c r="H21" s="1">
-        <v>2887</v>
+        <v>4870</v>
       </c>
       <c r="I21" s="1">
-        <v>1064</v>
+        <v>910</v>
       </c>
       <c r="J21" s="1">
-        <v>3496</v>
+        <v>5174</v>
       </c>
       <c r="K21" s="1">
-        <v>2066</v>
+        <v>1078</v>
       </c>
       <c r="L21" s="1">
-        <v>3698</v>
+        <v>3162</v>
       </c>
       <c r="M21" s="1">
-        <v>350</v>
+        <v>1328</v>
       </c>
       <c r="N21" s="1">
-        <v>5304</v>
+        <v>8732</v>
       </c>
       <c r="O21" s="1">
-        <v>4655</v>
+        <v>4329</v>
       </c>
       <c r="P21" s="1">
-        <v>14096</v>
+        <v>16095</v>
       </c>
       <c r="Q21" s="1">
-        <v>40</v>
+        <v>646</v>
       </c>
       <c r="R21" s="1">
-        <v>13730</v>
+        <v>13883</v>
       </c>
       <c r="S21" s="1">
-        <v>6697</v>
+        <v>3891</v>
       </c>
       <c r="T21" s="1">
-        <v>10976</v>
+        <v>7352</v>
       </c>
       <c r="U21" s="1">
-        <v>1989</v>
+        <v>5018</v>
       </c>
       <c r="V21" s="1">
-        <v>7396</v>
+        <v>4050</v>
       </c>
     </row>
     <row r="22" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A22" s="1">
-        <v>2013</v>
+        <v>2014</v>
       </c>
       <c r="B22" s="1">
-        <v>10583</v>
+        <v>29396</v>
       </c>
       <c r="C22" s="1">
-        <v>2297</v>
+        <v>7483</v>
       </c>
       <c r="D22" s="1">
-        <v>7848</v>
+        <v>44323</v>
       </c>
       <c r="E22" s="1">
-        <v>26946</v>
+        <v>47492</v>
       </c>
       <c r="F22" s="1">
-        <v>2207</v>
+        <v>1165</v>
       </c>
       <c r="G22" s="1">
-        <v>8883</v>
+        <v>42114</v>
       </c>
       <c r="H22" s="1">
-        <v>4870</v>
+        <v>15890</v>
       </c>
       <c r="I22" s="1">
-        <v>910</v>
+        <v>6529</v>
       </c>
       <c r="J22" s="1">
-        <v>5174</v>
+        <v>34858</v>
       </c>
       <c r="K22" s="1">
-        <v>1078</v>
+        <v>7261</v>
       </c>
       <c r="L22" s="1">
-        <v>3162</v>
+        <v>4536</v>
       </c>
       <c r="M22" s="1">
-        <v>1328</v>
+        <v>4195</v>
       </c>
       <c r="N22" s="1">
-        <v>8732</v>
+        <v>22225</v>
       </c>
       <c r="O22" s="1">
-        <v>4329</v>
+        <v>8183</v>
       </c>
       <c r="P22" s="1">
-        <v>16095</v>
+        <v>44341</v>
       </c>
       <c r="Q22" s="1">
-        <v>646</v>
+        <v>467</v>
       </c>
       <c r="R22" s="1">
-        <v>13883</v>
+        <v>13010</v>
       </c>
       <c r="S22" s="1">
-        <v>3891</v>
+        <v>4208</v>
       </c>
       <c r="T22" s="1">
-        <v>7352</v>
+        <v>12701</v>
       </c>
       <c r="U22" s="1">
-        <v>5018</v>
+        <v>22903</v>
       </c>
       <c r="V22" s="1">
-        <v>4050</v>
+        <v>29163</v>
       </c>
     </row>
     <row r="23" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A23" s="1">
-        <v>2014</v>
+        <v>2015</v>
       </c>
       <c r="B23" s="1">
-        <v>29396</v>
+        <v>7399</v>
       </c>
       <c r="C23" s="1">
-        <v>7483</v>
+        <v>398</v>
       </c>
       <c r="D23" s="1">
-        <v>44323</v>
+        <v>3636</v>
       </c>
       <c r="E23" s="1">
-        <v>47492</v>
+        <v>4028</v>
       </c>
       <c r="F23" s="1">
-        <v>1165</v>
+        <v>1902</v>
       </c>
       <c r="G23" s="1">
-        <v>42114</v>
+        <v>4470</v>
       </c>
       <c r="H23" s="1">
-        <v>15890</v>
+        <v>2694</v>
       </c>
       <c r="I23" s="1">
-        <v>6529</v>
+        <v>1016</v>
       </c>
       <c r="J23" s="1">
-        <v>34858</v>
+        <v>3695</v>
       </c>
       <c r="K23" s="1">
-        <v>7261</v>
+        <v>1235</v>
       </c>
       <c r="L23" s="1">
-        <v>4536</v>
+        <v>3594</v>
       </c>
       <c r="M23" s="1">
-        <v>4195</v>
+        <v>398</v>
       </c>
       <c r="N23" s="1">
-        <v>22225</v>
+        <v>2659</v>
       </c>
       <c r="O23" s="1">
-        <v>8183</v>
+        <v>1870</v>
       </c>
       <c r="P23" s="1">
-        <v>44341</v>
+        <v>12422</v>
       </c>
       <c r="Q23" s="1">
-        <v>467</v>
+        <v>202</v>
       </c>
       <c r="R23" s="1">
-        <v>13010</v>
+        <v>7054</v>
       </c>
       <c r="S23" s="1">
-        <v>4208</v>
+        <v>1302</v>
       </c>
       <c r="T23" s="1">
-        <v>12701</v>
+        <v>2503</v>
       </c>
       <c r="U23" s="1">
-        <v>22903</v>
+        <v>1614</v>
       </c>
       <c r="V23" s="1">
-        <v>29163</v>
+        <v>2880</v>
       </c>
     </row>
     <row r="24" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A24" s="1">
-        <v>2015</v>
+        <v>2016</v>
       </c>
       <c r="B24" s="1">
-        <v>7399</v>
+        <v>8039</v>
       </c>
       <c r="C24" s="1">
-        <v>398</v>
+        <v>1863</v>
       </c>
       <c r="D24" s="1">
-        <v>3636</v>
+        <v>5040</v>
       </c>
       <c r="E24" s="1">
-        <v>4028</v>
+        <v>10348</v>
       </c>
       <c r="F24" s="1">
-        <v>1902</v>
+        <v>1027</v>
       </c>
       <c r="G24" s="1">
-        <v>4470</v>
+        <v>4820</v>
       </c>
       <c r="H24" s="1">
-        <v>2694</v>
+        <v>1263</v>
       </c>
       <c r="I24" s="1">
-        <v>1016</v>
+        <v>1020</v>
       </c>
       <c r="J24" s="1">
-        <v>3695</v>
+        <v>8228</v>
       </c>
       <c r="K24" s="1">
-        <v>1235</v>
+        <v>2629</v>
       </c>
       <c r="L24" s="1">
-        <v>3594</v>
+        <v>1251</v>
       </c>
       <c r="M24" s="1">
-        <v>398</v>
+        <v>1149</v>
       </c>
       <c r="N24" s="1">
-        <v>2659</v>
+        <v>3286</v>
       </c>
       <c r="O24" s="1">
-        <v>1870</v>
+        <v>2639</v>
       </c>
       <c r="P24" s="1">
-        <v>12422</v>
+        <v>9964</v>
       </c>
       <c r="Q24" s="1">
-        <v>202</v>
+        <v>131</v>
       </c>
       <c r="R24" s="1">
-        <v>7054</v>
+        <v>834</v>
       </c>
       <c r="S24" s="1">
-        <v>1302</v>
+        <v>4768</v>
       </c>
       <c r="T24" s="1">
-        <v>2503</v>
+        <v>1361</v>
       </c>
       <c r="U24" s="1">
-        <v>1614</v>
+        <v>7741</v>
       </c>
       <c r="V24" s="1">
-        <v>2880</v>
+        <v>4066</v>
       </c>
     </row>
     <row r="25" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A25" s="1">
-        <v>2016</v>
+        <v>2017</v>
       </c>
       <c r="B25" s="1">
-        <v>8039</v>
+        <v>4931</v>
       </c>
       <c r="C25" s="1">
-        <v>1863</v>
+        <v>1786</v>
       </c>
       <c r="D25" s="1">
-        <v>5040</v>
+        <v>3092</v>
       </c>
       <c r="E25" s="1">
-        <v>10348</v>
+        <v>5337</v>
       </c>
       <c r="F25" s="1">
-        <v>1027</v>
+        <v>797</v>
       </c>
       <c r="G25" s="1">
-        <v>4820</v>
+        <v>12475</v>
       </c>
       <c r="H25" s="1">
-        <v>1263</v>
+        <v>2056</v>
       </c>
       <c r="I25" s="1">
-        <v>1020</v>
+        <v>608</v>
       </c>
       <c r="J25" s="1">
-        <v>8228</v>
+        <v>6309</v>
       </c>
       <c r="K25" s="1">
-        <v>2629</v>
+        <v>5169</v>
       </c>
       <c r="L25" s="1">
-        <v>1251</v>
+        <v>2038</v>
       </c>
       <c r="M25" s="1">
-        <v>1149</v>
+        <v>518</v>
       </c>
       <c r="N25" s="1">
-        <v>3286</v>
+        <v>5982</v>
       </c>
       <c r="O25" s="1">
-        <v>2639</v>
+        <v>822</v>
       </c>
       <c r="P25" s="1">
-        <v>9964</v>
+        <v>8198</v>
       </c>
       <c r="Q25" s="1">
-        <v>131</v>
+        <v>79</v>
       </c>
       <c r="R25" s="1">
-        <v>834</v>
+        <v>1247</v>
       </c>
       <c r="S25" s="1">
-        <v>4768</v>
+        <v>309</v>
       </c>
       <c r="T25" s="1">
-        <v>1361</v>
+        <v>366</v>
       </c>
       <c r="U25" s="1">
-        <v>7741</v>
+        <v>3366</v>
       </c>
       <c r="V25" s="1">
-        <v>4066</v>
+        <v>2865</v>
       </c>
     </row>
     <row r="26" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A26" s="1">
-        <v>2017</v>
+        <v>2018</v>
       </c>
       <c r="B26" s="1">
-        <v>4931</v>
+        <v>5720</v>
       </c>
       <c r="C26" s="1">
-        <v>1786</v>
+        <v>558</v>
       </c>
       <c r="D26" s="1">
-        <v>3092</v>
+        <v>8240</v>
       </c>
       <c r="E26" s="1">
-        <v>5337</v>
+        <v>6427</v>
       </c>
       <c r="F26" s="1">
-        <v>797</v>
+        <v>710</v>
       </c>
       <c r="G26" s="1">
-        <v>12475</v>
+        <v>15910</v>
       </c>
       <c r="H26" s="1">
-        <v>2056</v>
+        <v>4393</v>
       </c>
       <c r="I26" s="1">
-        <v>608</v>
+        <v>444</v>
       </c>
       <c r="J26" s="1">
-        <v>6309</v>
+        <v>4735</v>
       </c>
       <c r="K26" s="1">
-        <v>5169</v>
+        <v>1211</v>
       </c>
       <c r="L26" s="1">
-        <v>2038</v>
+        <v>3324</v>
       </c>
       <c r="M26" s="1">
-        <v>518</v>
+        <v>116</v>
       </c>
       <c r="N26" s="1">
-        <v>5982</v>
+        <v>4592</v>
       </c>
       <c r="O26" s="1">
-        <v>822</v>
+        <v>2549</v>
       </c>
       <c r="P26" s="1">
-        <v>8198</v>
+        <v>7498</v>
       </c>
       <c r="Q26" s="1">
-        <v>79</v>
+        <v>197</v>
       </c>
       <c r="R26" s="1">
-        <v>1247</v>
+        <v>3531</v>
       </c>
       <c r="S26" s="1">
-        <v>309</v>
+        <v>1939</v>
       </c>
       <c r="T26" s="1">
-        <v>366</v>
+        <v>3130</v>
       </c>
       <c r="U26" s="1">
-        <v>3366</v>
+        <v>2300</v>
       </c>
       <c r="V26" s="1">
-        <v>2865</v>
+        <v>5279</v>
       </c>
     </row>
     <row r="27" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A27" s="1">
-        <v>2018</v>
+        <v>2019</v>
       </c>
       <c r="B27" s="1">
-        <v>5720</v>
+        <v>5432</v>
       </c>
       <c r="C27" s="1">
-        <v>558</v>
+        <v>912</v>
       </c>
       <c r="D27" s="1">
-        <v>8240</v>
+        <v>14884</v>
       </c>
       <c r="E27" s="1">
-        <v>6427</v>
+        <v>13262</v>
       </c>
       <c r="F27" s="1">
-        <v>710</v>
+        <v>1012</v>
       </c>
       <c r="G27" s="1">
-        <v>15910</v>
+        <v>10250</v>
       </c>
       <c r="H27" s="1">
-        <v>4393</v>
+        <v>3476</v>
       </c>
       <c r="I27" s="1">
-        <v>444</v>
+        <v>782</v>
       </c>
       <c r="J27" s="1">
-        <v>4735</v>
+        <v>13869</v>
       </c>
       <c r="K27" s="1">
-        <v>1211</v>
+        <v>5154</v>
       </c>
       <c r="L27" s="1">
-        <v>3324</v>
+        <v>3698</v>
       </c>
       <c r="M27" s="1">
-        <v>116</v>
+        <v>241</v>
       </c>
       <c r="N27" s="1">
-        <v>4592</v>
+        <v>5050</v>
       </c>
       <c r="O27" s="1">
-        <v>2549</v>
+        <v>1193</v>
       </c>
       <c r="P27" s="1">
-        <v>7498</v>
+        <v>6587</v>
       </c>
       <c r="Q27" s="1">
-        <v>197</v>
+        <v>174</v>
       </c>
       <c r="R27" s="1">
-        <v>3531</v>
+        <v>4032</v>
       </c>
       <c r="S27" s="1">
-        <v>1939</v>
+        <v>1574</v>
       </c>
       <c r="T27" s="1">
-        <v>3130</v>
+        <v>5559</v>
       </c>
       <c r="U27" s="1">
-        <v>2300</v>
+        <v>4436</v>
       </c>
       <c r="V27" s="1">
-        <v>5279</v>
+        <v>3866</v>
       </c>
     </row>
     <row r="28" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A28" s="1">
-        <v>2019</v>
+        <v>2016</v>
       </c>
       <c r="B28" s="1">
-        <v>5432</v>
+        <v>8039</v>
       </c>
       <c r="C28" s="1">
-        <v>912</v>
+        <v>1863</v>
       </c>
       <c r="D28" s="1">
-        <v>14884</v>
+        <v>5040</v>
       </c>
       <c r="E28" s="1">
-        <v>13262</v>
+        <v>10348</v>
       </c>
       <c r="F28" s="1">
-        <v>1012</v>
+        <v>1027</v>
       </c>
       <c r="G28" s="1">
-        <v>10250</v>
+        <v>4820</v>
       </c>
       <c r="H28" s="1">
-        <v>3476</v>
+        <v>1263</v>
       </c>
       <c r="I28" s="1">
-        <v>782</v>
+        <v>1020</v>
       </c>
       <c r="J28" s="1">
-        <v>13869</v>
+        <v>8228</v>
       </c>
       <c r="K28" s="1">
-        <v>5154</v>
+        <v>2629</v>
       </c>
       <c r="L28" s="1">
-        <v>3698</v>
+        <v>1251</v>
       </c>
       <c r="M28" s="1">
-        <v>241</v>
+        <v>1149</v>
       </c>
       <c r="N28" s="1">
-        <v>5050</v>
+        <v>3286</v>
       </c>
       <c r="O28" s="1">
-        <v>1193</v>
+        <v>2639</v>
       </c>
       <c r="P28" s="1">
-        <v>6587</v>
+        <v>9964</v>
       </c>
       <c r="Q28" s="1">
-        <v>174</v>
+        <v>131</v>
       </c>
       <c r="R28" s="1">
-        <v>4032</v>
+        <v>834</v>
       </c>
       <c r="S28" s="1">
-        <v>1574</v>
+        <v>4768</v>
       </c>
       <c r="T28" s="1">
-        <v>5559</v>
+        <v>1361</v>
       </c>
       <c r="U28" s="1">
-        <v>4436</v>
+        <v>7741</v>
       </c>
       <c r="V28" s="1">
-        <v>3866</v>
+        <v>4066</v>
       </c>
     </row>
     <row r="29" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A29" s="1">
-        <v>2016</v>
+        <v>2017</v>
       </c>
       <c r="B29" s="1">
-        <v>8039</v>
+        <v>4931</v>
       </c>
       <c r="C29" s="1">
-        <v>1863</v>
+        <v>1786</v>
       </c>
       <c r="D29" s="1">
-        <v>5040</v>
+        <v>3092</v>
       </c>
       <c r="E29" s="1">
-        <v>10348</v>
+        <v>5337</v>
       </c>
       <c r="F29" s="1">
-        <v>1027</v>
+        <v>797</v>
       </c>
       <c r="G29" s="1">
-        <v>4820</v>
+        <v>12475</v>
       </c>
       <c r="H29" s="1">
-        <v>1263</v>
+        <v>2056</v>
       </c>
       <c r="I29" s="1">
-        <v>1020</v>
+        <v>608</v>
       </c>
       <c r="J29" s="1">
-        <v>8228</v>
+        <v>6309</v>
       </c>
       <c r="K29" s="1">
-        <v>2629</v>
+        <v>5169</v>
       </c>
       <c r="L29" s="1">
-        <v>1251</v>
+        <v>2038</v>
       </c>
       <c r="M29" s="1">
-        <v>1149</v>
+        <v>518</v>
       </c>
       <c r="N29" s="1">
-        <v>3286</v>
+        <v>5982</v>
       </c>
       <c r="O29" s="1">
-        <v>2639</v>
+        <v>822</v>
       </c>
       <c r="P29" s="1">
-        <v>9964</v>
+        <v>8198</v>
       </c>
       <c r="Q29" s="1">
-        <v>131</v>
+        <v>79</v>
       </c>
       <c r="R29" s="1">
-        <v>834</v>
+        <v>1247</v>
       </c>
       <c r="S29" s="1">
-        <v>4768</v>
+        <v>309</v>
       </c>
       <c r="T29" s="1">
-        <v>1361</v>
+        <v>366</v>
       </c>
       <c r="U29" s="1">
-        <v>7741</v>
+        <v>3366</v>
       </c>
       <c r="V29" s="1">
-        <v>4066</v>
+        <v>2865</v>
       </c>
     </row>
     <row r="30" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A30" s="1">
-        <v>2017</v>
+        <v>2018</v>
       </c>
       <c r="B30" s="1">
-        <v>4931</v>
+        <v>5720</v>
       </c>
       <c r="C30" s="1">
-        <v>1786</v>
+        <v>558</v>
       </c>
       <c r="D30" s="1">
-        <v>3092</v>
+        <v>8240</v>
       </c>
       <c r="E30" s="1">
-        <v>5337</v>
+        <v>6427</v>
       </c>
       <c r="F30" s="1">
-        <v>797</v>
+        <v>710</v>
       </c>
       <c r="G30" s="1">
-        <v>12475</v>
+        <v>15910</v>
       </c>
       <c r="H30" s="1">
-        <v>2056</v>
+        <v>4393</v>
       </c>
       <c r="I30" s="1">
-        <v>608</v>
+        <v>444</v>
       </c>
       <c r="J30" s="1">
-        <v>6309</v>
+        <v>4735</v>
       </c>
       <c r="K30" s="1">
-        <v>5169</v>
+        <v>1211</v>
       </c>
       <c r="L30" s="1">
-        <v>2038</v>
+        <v>3324</v>
       </c>
       <c r="M30" s="1">
-        <v>518</v>
+        <v>116</v>
       </c>
       <c r="N30" s="1">
-        <v>5982</v>
+        <v>4592</v>
       </c>
       <c r="O30" s="1">
-        <v>822</v>
+        <v>2549</v>
       </c>
       <c r="P30" s="1">
-        <v>8198</v>
+        <v>7498</v>
       </c>
       <c r="Q30" s="1">
-        <v>79</v>
+        <v>197</v>
       </c>
       <c r="R30" s="1">
-        <v>1247</v>
+        <v>3531</v>
       </c>
       <c r="S30" s="1">
-        <v>309</v>
+        <v>1939</v>
       </c>
       <c r="T30" s="1">
-        <v>366</v>
+        <v>3130</v>
       </c>
       <c r="U30" s="1">
-        <v>3366</v>
+        <v>2300</v>
       </c>
       <c r="V30" s="1">
-        <v>2865</v>
+        <v>5279</v>
       </c>
     </row>
     <row r="31" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A31" s="1">
-        <v>2018</v>
+        <v>2019</v>
       </c>
       <c r="B31" s="1">
-        <v>5720</v>
+        <v>5432</v>
       </c>
       <c r="C31" s="1">
-        <v>558</v>
+        <v>912</v>
       </c>
       <c r="D31" s="1">
-        <v>8240</v>
+        <v>14884</v>
       </c>
       <c r="E31" s="1">
-        <v>6427</v>
+        <v>13262</v>
       </c>
       <c r="F31" s="1">
-        <v>710</v>
+        <v>1012</v>
       </c>
       <c r="G31" s="1">
-        <v>15910</v>
+        <v>10250</v>
       </c>
       <c r="H31" s="1">
-        <v>4393</v>
+        <v>3476</v>
       </c>
       <c r="I31" s="1">
-        <v>444</v>
+        <v>782</v>
       </c>
       <c r="J31" s="1">
-        <v>4735</v>
+        <v>13869</v>
       </c>
       <c r="K31" s="1">
-        <v>1211</v>
+        <v>5154</v>
       </c>
       <c r="L31" s="1">
-        <v>3324</v>
+        <v>3698</v>
       </c>
       <c r="M31" s="1">
-        <v>116</v>
+        <v>241</v>
       </c>
       <c r="N31" s="1">
-        <v>4592</v>
+        <v>5050</v>
       </c>
       <c r="O31" s="1">
-        <v>2549</v>
+        <v>1193</v>
       </c>
       <c r="P31" s="1">
-        <v>7498</v>
+        <v>6587</v>
       </c>
       <c r="Q31" s="1">
-        <v>197</v>
+        <v>174</v>
       </c>
       <c r="R31" s="1">
-        <v>3531</v>
+        <v>4032</v>
       </c>
       <c r="S31" s="1">
-        <v>1939</v>
+        <v>1574</v>
       </c>
       <c r="T31" s="1">
-        <v>3130</v>
+        <v>5559</v>
       </c>
       <c r="U31" s="1">
-        <v>2300</v>
+        <v>4436</v>
       </c>
       <c r="V31" s="1">
-        <v>5279</v>
-      </c>
-    </row>
-    <row r="32" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A32" s="1">
-        <v>2019</v>
-      </c>
-      <c r="B32" s="1">
-        <v>5432</v>
-      </c>
-      <c r="C32" s="1">
-        <v>912</v>
-      </c>
-      <c r="D32" s="1">
-        <v>14884</v>
-      </c>
-      <c r="E32" s="1">
-        <v>13262</v>
-      </c>
-      <c r="F32" s="1">
-        <v>1012</v>
-      </c>
-      <c r="G32" s="1">
-        <v>10250</v>
-      </c>
-      <c r="H32" s="1">
-        <v>3476</v>
-      </c>
-      <c r="I32" s="1">
-        <v>782</v>
-      </c>
-      <c r="J32" s="1">
-        <v>13869</v>
-      </c>
-      <c r="K32" s="1">
-        <v>5154</v>
-      </c>
-      <c r="L32" s="1">
-        <v>3698</v>
-      </c>
-      <c r="M32" s="1">
-        <v>241</v>
-      </c>
-      <c r="N32" s="1">
-        <v>5050</v>
-      </c>
-      <c r="O32" s="1">
-        <v>1193</v>
-      </c>
-      <c r="P32" s="1">
-        <v>6587</v>
-      </c>
-      <c r="Q32" s="1">
-        <v>174</v>
-      </c>
-      <c r="R32" s="1">
-        <v>4032</v>
-      </c>
-      <c r="S32" s="1">
-        <v>1574</v>
-      </c>
-      <c r="T32" s="1">
-        <v>5559</v>
-      </c>
-      <c r="U32" s="1">
-        <v>4436</v>
-      </c>
-      <c r="V32" s="1">
         <v>3866</v>
       </c>
     </row>

</xml_diff>